<commit_message>
alteracoes durante a producao do artigo
</commit_message>
<xml_diff>
--- a/reports/tables/TCC_comparacao_GR_RZ.xlsx
+++ b/reports/tables/TCC_comparacao_GR_RZ.xlsx
@@ -425,7 +425,7 @@
     <outlinePr summaryBelow="1" summaryRight="1"/>
     <pageSetUpPr/>
   </sheetPr>
-  <dimension ref="A1:N58"/>
+  <dimension ref="A1:N81"/>
   <sheetViews>
     <sheetView workbookViewId="0">
       <selection activeCell="A1" sqref="A1"/>
@@ -549,10 +549,10 @@
         </is>
       </c>
       <c r="M2" t="n">
-        <v>-0.8153725592639325</v>
+        <v>-0.9040691591397625</v>
       </c>
       <c r="N2" t="n">
-        <v>-1.153206573162285</v>
+        <v>-1.331650096687082</v>
       </c>
     </row>
     <row r="3">
@@ -601,10 +601,10 @@
         </is>
       </c>
       <c r="M3" t="n">
-        <v>-0.9493246517171932</v>
+        <v>-0.9938680374151502</v>
       </c>
       <c r="N3" t="n">
-        <v>-0.3775346710980368</v>
+        <v>-0.5678070066536358</v>
       </c>
     </row>
     <row r="4">
@@ -620,32 +620,32 @@
       </c>
       <c r="C4" t="inlineStr">
         <is>
-          <t>trial_02</t>
+          <t>trial_03</t>
         </is>
       </c>
       <c r="D4" t="n">
         <v>6</v>
       </c>
       <c r="E4" t="n">
-        <v>-0.08433924684844755</v>
+        <v>0.05400249968757712</v>
       </c>
       <c r="F4" t="n">
-        <v>0.4401794406596365</v>
+        <v>0.6014934886745595</v>
       </c>
       <c r="G4" t="n">
-        <v>0.9</v>
+        <v>0.9166666666666666</v>
       </c>
       <c r="H4" t="n">
-        <v>0.6931923967221079</v>
+        <v>0.6928170294222846</v>
       </c>
       <c r="I4" t="n">
-        <v>0.826117542733139</v>
+        <v>0.8148063333636306</v>
       </c>
       <c r="J4" t="n">
-        <v>0.7491220886027253</v>
+        <v>0.7382672229016439</v>
       </c>
       <c r="K4" t="n">
-        <v>0.4562647754137116</v>
+        <v>0.4657210401891253</v>
       </c>
       <c r="L4" t="inlineStr">
         <is>
@@ -653,10 +653,10 @@
         </is>
       </c>
       <c r="M4" t="n">
-        <v>-0.2275080617898399</v>
+        <v>1.404626357021766</v>
       </c>
       <c r="N4" t="n">
-        <v>-0.3138199735775747</v>
+        <v>-0.5720650348413162</v>
       </c>
     </row>
     <row r="5">
@@ -672,32 +672,32 @@
       </c>
       <c r="C5" t="inlineStr">
         <is>
-          <t>trial_03</t>
+          <t>trial_04</t>
         </is>
       </c>
       <c r="D5" t="n">
-        <v>7</v>
+        <v>5</v>
       </c>
       <c r="E5" t="n">
-        <v>-0.0817047848124746</v>
+        <v>-0.05449293067472025</v>
       </c>
       <c r="F5" t="n">
-        <v>0.4708200322014888</v>
+        <v>0.653725620375568</v>
       </c>
       <c r="G5" t="n">
-        <v>0.9142857142857143</v>
+        <v>0.86</v>
       </c>
       <c r="H5" t="n">
-        <v>0.6956458845119702</v>
+        <v>0.6953156172051727</v>
       </c>
       <c r="I5" t="n">
-        <v>0.9086885508754189</v>
+        <v>0.8178113197355633</v>
       </c>
       <c r="J5" t="n">
-        <v>0.7548030569464876</v>
+        <v>0.7766163965983484</v>
       </c>
       <c r="K5" t="n">
-        <v>0.5271867612293144</v>
+        <v>0.5035460992907801</v>
       </c>
       <c r="L5" t="inlineStr">
         <is>
@@ -705,10 +705,10 @@
         </is>
       </c>
       <c r="M5" t="n">
-        <v>-0.02727245525669855</v>
+        <v>0.8235437044100925</v>
       </c>
       <c r="N5" t="n">
-        <v>0.1187883041707768</v>
+        <v>-0.3617157171643979</v>
       </c>
     </row>
     <row r="6">
@@ -724,32 +724,32 @@
       </c>
       <c r="C6" t="inlineStr">
         <is>
-          <t>trial_04</t>
+          <t>trial_09</t>
         </is>
       </c>
       <c r="D6" t="n">
         <v>5</v>
       </c>
       <c r="E6" t="n">
-        <v>-0.1910851157195024</v>
+        <v>-0.1571832061258721</v>
       </c>
       <c r="F6" t="n">
-        <v>0.43890969558159</v>
+        <v>0.485382021413221</v>
       </c>
       <c r="G6" t="n">
-        <v>0.86</v>
+        <v>0.88</v>
       </c>
       <c r="H6" t="n">
-        <v>0.6975202568033627</v>
+        <v>0.6985559268412986</v>
       </c>
       <c r="I6" t="n">
-        <v>0.783640476776861</v>
+        <v>0.7289716451650452</v>
       </c>
       <c r="J6" t="n">
-        <v>0.8043093151913384</v>
+        <v>0.715388141509927</v>
       </c>
       <c r="K6" t="n">
-        <v>0.5508274231678487</v>
+        <v>0.4468085106382979</v>
       </c>
       <c r="L6" t="inlineStr">
         <is>
@@ -757,10 +757,10 @@
         </is>
       </c>
       <c r="M6" t="n">
-        <v>-1.012443229590916</v>
+        <v>-0.5709409316920336</v>
       </c>
       <c r="N6" t="n">
-        <v>-0.2529522765955518</v>
+        <v>-1.130282823057612</v>
       </c>
     </row>
     <row r="7">
@@ -776,32 +776,32 @@
       </c>
       <c r="C7" t="inlineStr">
         <is>
-          <t>trial_05</t>
+          <t>trial_10</t>
         </is>
       </c>
       <c r="D7" t="n">
         <v>5</v>
       </c>
       <c r="E7" t="n">
-        <v>-0.1000172106736911</v>
+        <v>-0.1571832061258721</v>
       </c>
       <c r="F7" t="n">
-        <v>0.5097918707047079</v>
+        <v>0.485382021413221</v>
       </c>
       <c r="G7" t="n">
-        <v>0.86</v>
+        <v>0.88</v>
       </c>
       <c r="H7" t="n">
-        <v>0.6944291444867012</v>
+        <v>0.6985559268412986</v>
       </c>
       <c r="I7" t="n">
-        <v>0.7493112739992964</v>
+        <v>0.7289716451650452</v>
       </c>
       <c r="J7" t="n">
-        <v>0.7624164859238228</v>
+        <v>0.715388141509927</v>
       </c>
       <c r="K7" t="n">
-        <v>0.4988179669030733</v>
+        <v>0.4468085106382979</v>
       </c>
       <c r="L7" t="inlineStr">
         <is>
@@ -809,10 +809,10 @@
         </is>
       </c>
       <c r="M7" t="n">
-        <v>-0.1010686900994924</v>
+        <v>-0.5709409316920336</v>
       </c>
       <c r="N7" t="n">
-        <v>-0.6146177490962569</v>
+        <v>-1.130282823057612</v>
       </c>
     </row>
     <row r="8">
@@ -828,32 +828,32 @@
       </c>
       <c r="C8" t="inlineStr">
         <is>
-          <t>trial_09</t>
+          <t>trial_15</t>
         </is>
       </c>
       <c r="D8" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E8" t="n">
-        <v>-0.1571832061258721</v>
+        <v>0.04678469130341358</v>
       </c>
       <c r="F8" t="n">
-        <v>0.485382021413221</v>
+        <v>0.6065677393203338</v>
       </c>
       <c r="G8" t="n">
-        <v>0.88</v>
+        <v>0.9428571428571428</v>
       </c>
       <c r="H8" t="n">
-        <v>0.6985559268412986</v>
+        <v>0.6991037719646418</v>
       </c>
       <c r="I8" t="n">
-        <v>0.7289716451650452</v>
+        <v>0.874752117833566</v>
       </c>
       <c r="J8" t="n">
-        <v>0.715388141509927</v>
+        <v>0.7168282334553895</v>
       </c>
       <c r="K8" t="n">
-        <v>0.4468085106382979</v>
+        <v>0.5484633569739953</v>
       </c>
       <c r="L8" t="inlineStr">
         <is>
@@ -861,10 +861,10 @@
         </is>
       </c>
       <c r="M8" t="n">
-        <v>-0.5246273498383018</v>
+        <v>1.455581313081372</v>
       </c>
       <c r="N8" t="n">
-        <v>-0.8858178755216501</v>
+        <v>-0.2811240374019704</v>
       </c>
     </row>
     <row r="9">
@@ -880,32 +880,32 @@
       </c>
       <c r="C9" t="inlineStr">
         <is>
-          <t>trial_10</t>
+          <t>trial_16</t>
         </is>
       </c>
       <c r="D9" t="n">
-        <v>5</v>
+        <v>7</v>
       </c>
       <c r="E9" t="n">
-        <v>-0.1571832061258721</v>
+        <v>0.0659744857413915</v>
       </c>
       <c r="F9" t="n">
-        <v>0.485382021413221</v>
+        <v>0.6412702717792301</v>
       </c>
       <c r="G9" t="n">
-        <v>0.88</v>
+        <v>0.9</v>
       </c>
       <c r="H9" t="n">
-        <v>0.6985559268412986</v>
+        <v>0.7767928482604098</v>
       </c>
       <c r="I9" t="n">
-        <v>0.7289716451650452</v>
+        <v>0.874752117833566</v>
       </c>
       <c r="J9" t="n">
-        <v>0.715388141509927</v>
+        <v>0.7168282334553895</v>
       </c>
       <c r="K9" t="n">
-        <v>0.4468085106382979</v>
+        <v>0.5484633569739953</v>
       </c>
       <c r="L9" t="inlineStr">
         <is>
@@ -913,10 +913,10 @@
         </is>
       </c>
       <c r="M9" t="n">
-        <v>-0.5246273498383018</v>
+        <v>1.624769447895308</v>
       </c>
       <c r="N9" t="n">
-        <v>-0.8858178755216501</v>
+        <v>0.2647201368017852</v>
       </c>
     </row>
     <row r="10">
@@ -927,37 +927,37 @@
       </c>
       <c r="B10" t="inlineStr">
         <is>
-          <t>run_UNGROUPED</t>
+          <t>run_20250831T230602Z</t>
         </is>
       </c>
       <c r="C10" t="inlineStr">
         <is>
-          <t>trial_15</t>
+          <t>trial_02</t>
         </is>
       </c>
       <c r="D10" t="n">
-        <v>7</v>
+        <v>6</v>
       </c>
       <c r="E10" t="n">
-        <v>0.04678469130341358</v>
+        <v>-0.1036481696278762</v>
       </c>
       <c r="F10" t="n">
-        <v>0.6065677393203338</v>
+        <v>0.6505978159772585</v>
       </c>
       <c r="G10" t="n">
-        <v>0.9428571428571428</v>
+        <v>0.9166666666666666</v>
       </c>
       <c r="H10" t="n">
-        <v>0.6991037719646418</v>
+        <v>0.7964118694248346</v>
       </c>
       <c r="I10" t="n">
-        <v>0.874752117833566</v>
+        <v>0.8359601236154192</v>
       </c>
       <c r="J10" t="n">
-        <v>0.7168282334553895</v>
+        <v>0.6491606370470357</v>
       </c>
       <c r="K10" t="n">
-        <v>0.5484633569739953</v>
+        <v>0.5011820330969267</v>
       </c>
       <c r="L10" t="inlineStr">
         <is>
@@ -965,10 +965,10 @@
         </is>
       </c>
       <c r="M10" t="n">
-        <v>1.504325224652445</v>
+        <v>0.6567837702910052</v>
       </c>
       <c r="N10" t="n">
-        <v>-0.1827125851258963</v>
+        <v>-0.1303003447728534</v>
       </c>
     </row>
     <row r="11">
@@ -979,48 +979,44 @@
       </c>
       <c r="B11" t="inlineStr">
         <is>
-          <t>run_UNGROUPED</t>
+          <t>run_20250831T230602Z</t>
         </is>
       </c>
       <c r="C11" t="inlineStr">
         <is>
-          <t>trial_16</t>
+          <t>trial_03</t>
         </is>
       </c>
       <c r="D11" t="n">
-        <v>7</v>
-      </c>
-      <c r="E11" t="n">
-        <v>0.0659744857413915</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="E11" t="inlineStr"/>
       <c r="F11" t="n">
-        <v>0.6412702717792301</v>
+        <v>0.5026942135711703</v>
       </c>
       <c r="G11" t="n">
-        <v>0.9</v>
+        <v>0.89375</v>
       </c>
       <c r="H11" t="n">
-        <v>0.7767928482604098</v>
+        <v>0.7431078485521072</v>
       </c>
       <c r="I11" t="n">
-        <v>0.874752117833566</v>
+        <v>0.9527068843159245</v>
       </c>
       <c r="J11" t="n">
-        <v>0.7168282334553895</v>
+        <v>0.6259126435805692</v>
       </c>
       <c r="K11" t="n">
-        <v>0.5484633569739953</v>
+        <v>0.2293144208037825</v>
       </c>
       <c r="L11" t="inlineStr">
         <is>
           <t>opt</t>
         </is>
       </c>
-      <c r="M11" t="n">
-        <v>1.676907334097042</v>
-      </c>
+      <c r="M11" t="inlineStr"/>
       <c r="N11" t="n">
-        <v>0.3105413786693814</v>
+        <v>0.06046960019251917</v>
       </c>
     </row>
     <row r="12">
@@ -1036,43 +1032,39 @@
       </c>
       <c r="C12" t="inlineStr">
         <is>
-          <t>trial_02</t>
+          <t>trial_04</t>
         </is>
       </c>
       <c r="D12" t="n">
-        <v>6</v>
-      </c>
-      <c r="E12" t="n">
-        <v>-0.1036481696278762</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="E12" t="inlineStr"/>
       <c r="F12" t="n">
-        <v>0.6505978159772585</v>
+        <v>0.5007400549962517</v>
       </c>
       <c r="G12" t="n">
-        <v>0.9166666666666666</v>
+        <v>0.896875</v>
       </c>
       <c r="H12" t="n">
-        <v>0.7964118694248346</v>
+        <v>0.7407559591321291</v>
       </c>
       <c r="I12" t="n">
-        <v>0.8359601236154192</v>
+        <v>0.9527068843159245</v>
       </c>
       <c r="J12" t="n">
-        <v>0.6491606370470357</v>
+        <v>0.6259126435805692</v>
       </c>
       <c r="K12" t="n">
-        <v>0.5011820330969267</v>
+        <v>0.2293144208037825</v>
       </c>
       <c r="L12" t="inlineStr">
         <is>
           <t>opt</t>
         </is>
       </c>
-      <c r="M12" t="n">
-        <v>0.6960934920475926</v>
-      </c>
+      <c r="M12" t="inlineStr"/>
       <c r="N12" t="n">
-        <v>-0.03813264239056893</v>
+        <v>0.04394520320549476</v>
       </c>
     </row>
     <row r="13">
@@ -1088,30 +1080,30 @@
       </c>
       <c r="C13" t="inlineStr">
         <is>
-          <t>trial_03</t>
+          <t>trial_06</t>
         </is>
       </c>
       <c r="D13" t="n">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="E13" t="inlineStr"/>
       <c r="F13" t="n">
-        <v>0.5026942135711703</v>
+        <v>0.558908702247524</v>
       </c>
       <c r="G13" t="n">
-        <v>0.89375</v>
+        <v>0.7631578947368421</v>
       </c>
       <c r="H13" t="n">
-        <v>0.7431078485521072</v>
+        <v>0.7887656388684514</v>
       </c>
       <c r="I13" t="n">
-        <v>0.9527068843159245</v>
+        <v>0.9409809457188111</v>
       </c>
       <c r="J13" t="n">
-        <v>0.6259126435805692</v>
+        <v>0.6739024108489315</v>
       </c>
       <c r="K13" t="n">
-        <v>0.2293144208037825</v>
+        <v>0.1134751773049645</v>
       </c>
       <c r="L13" t="inlineStr">
         <is>
@@ -1120,7 +1112,7 @@
       </c>
       <c r="M13" t="inlineStr"/>
       <c r="N13" t="n">
-        <v>0.07961759065271459</v>
+        <v>0.5334247590051294</v>
       </c>
     </row>
     <row r="14">
@@ -1136,39 +1128,43 @@
       </c>
       <c r="C14" t="inlineStr">
         <is>
-          <t>trial_04</t>
+          <t>trial_08</t>
         </is>
       </c>
       <c r="D14" t="n">
-        <v>32</v>
-      </c>
-      <c r="E14" t="inlineStr"/>
+        <v>10</v>
+      </c>
+      <c r="E14" t="n">
+        <v>-0.1269186739747705</v>
+      </c>
       <c r="F14" t="n">
-        <v>0.5007400549962517</v>
+        <v>0.430632870018162</v>
       </c>
       <c r="G14" t="n">
-        <v>0.896875</v>
+        <v>0.9</v>
       </c>
       <c r="H14" t="n">
-        <v>0.7407559591321291</v>
+        <v>0.6918583364919813</v>
       </c>
       <c r="I14" t="n">
-        <v>0.9527068843159245</v>
+        <v>0.8905002772962636</v>
       </c>
       <c r="J14" t="n">
-        <v>0.6259126435805692</v>
+        <v>0.6910758251167218</v>
       </c>
       <c r="K14" t="n">
-        <v>0.2293144208037825</v>
+        <v>0.2340425531914894</v>
       </c>
       <c r="L14" t="inlineStr">
         <is>
           <t>opt</t>
         </is>
       </c>
-      <c r="M14" t="inlineStr"/>
+      <c r="M14" t="n">
+        <v>-0.590336971284246</v>
+      </c>
       <c r="N14" t="n">
-        <v>0.06468526252982804</v>
+        <v>-0.3592829448266834</v>
       </c>
     </row>
     <row r="15">
@@ -1184,39 +1180,43 @@
       </c>
       <c r="C15" t="inlineStr">
         <is>
-          <t>trial_06</t>
+          <t>trial_09</t>
         </is>
       </c>
       <c r="D15" t="n">
-        <v>19</v>
-      </c>
-      <c r="E15" t="inlineStr"/>
+        <v>10</v>
+      </c>
+      <c r="E15" t="n">
+        <v>-0.1444746520885362</v>
+      </c>
       <c r="F15" t="n">
-        <v>0.558908702247524</v>
+        <v>0.4992851754818227</v>
       </c>
       <c r="G15" t="n">
-        <v>0.7631578947368421</v>
+        <v>0.88</v>
       </c>
       <c r="H15" t="n">
-        <v>0.7887656388684514</v>
+        <v>0.7960405662499628</v>
       </c>
       <c r="I15" t="n">
-        <v>0.9409809457188111</v>
+        <v>0.9274753131381483</v>
       </c>
       <c r="J15" t="n">
-        <v>0.6739024108489315</v>
+        <v>0.681657115384679</v>
       </c>
       <c r="K15" t="n">
-        <v>0.1134751773049645</v>
+        <v>0.293144208037825</v>
       </c>
       <c r="L15" t="inlineStr">
         <is>
           <t>opt</t>
         </is>
       </c>
-      <c r="M15" t="inlineStr"/>
+      <c r="M15" t="n">
+        <v>-0.4248784249228251</v>
+      </c>
       <c r="N15" t="n">
-        <v>0.5184686686776847</v>
+        <v>0.5423260228329674</v>
       </c>
     </row>
     <row r="16">
@@ -1232,32 +1232,32 @@
       </c>
       <c r="C16" t="inlineStr">
         <is>
-          <t>trial_08</t>
+          <t>trial_12</t>
         </is>
       </c>
       <c r="D16" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E16" t="n">
-        <v>-0.1269186739747705</v>
+        <v>-0.21965074556432</v>
       </c>
       <c r="F16" t="n">
-        <v>0.430632870018162</v>
+        <v>0.3864499959296761</v>
       </c>
       <c r="G16" t="n">
-        <v>0.9</v>
+        <v>0.8888888888888888</v>
       </c>
       <c r="H16" t="n">
-        <v>0.6918583364919813</v>
+        <v>0.6968434751923678</v>
       </c>
       <c r="I16" t="n">
-        <v>0.8905002772962636</v>
+        <v>0.9259782590668009</v>
       </c>
       <c r="J16" t="n">
-        <v>0.6910758251167218</v>
+        <v>0.7350611883314511</v>
       </c>
       <c r="K16" t="n">
-        <v>0.2340425531914894</v>
+        <v>0.4373522458628842</v>
       </c>
       <c r="L16" t="inlineStr">
         <is>
@@ -1265,10 +1265,10 @@
         </is>
       </c>
       <c r="M16" t="n">
-        <v>-0.5413613780400713</v>
+        <v>-1.411503453159859</v>
       </c>
       <c r="N16" t="n">
-        <v>-0.2636717594611607</v>
+        <v>0.08115795083589994</v>
       </c>
     </row>
     <row r="17">
@@ -1284,32 +1284,32 @@
       </c>
       <c r="C17" t="inlineStr">
         <is>
-          <t>trial_09</t>
+          <t>trial_14</t>
         </is>
       </c>
       <c r="D17" t="n">
         <v>10</v>
       </c>
       <c r="E17" t="n">
-        <v>-0.1444746520885362</v>
+        <v>-0.2064353951189201</v>
       </c>
       <c r="F17" t="n">
-        <v>0.4992851754818227</v>
+        <v>0.4852884006919144</v>
       </c>
       <c r="G17" t="n">
-        <v>0.88</v>
+        <v>0.92</v>
       </c>
       <c r="H17" t="n">
-        <v>0.7960405662499628</v>
+        <v>0.7760875846081373</v>
       </c>
       <c r="I17" t="n">
-        <v>0.9274753131381483</v>
+        <v>0.9237000216296234</v>
       </c>
       <c r="J17" t="n">
-        <v>0.681657115384679</v>
+        <v>0.702004565930465</v>
       </c>
       <c r="K17" t="n">
-        <v>0.293144208037825</v>
+        <v>0.3120567375886525</v>
       </c>
       <c r="L17" t="inlineStr">
         <is>
@@ -1317,10 +1317,10 @@
         </is>
       </c>
       <c r="M17" t="n">
-        <v>-0.3783576295641635</v>
+        <v>-0.7693122561303717</v>
       </c>
       <c r="N17" t="n">
-        <v>0.5334961934875875</v>
+        <v>0.4735362393898789</v>
       </c>
     </row>
     <row r="18">
@@ -1336,43 +1336,39 @@
       </c>
       <c r="C18" t="inlineStr">
         <is>
-          <t>trial_12</t>
+          <t>trial_15</t>
         </is>
       </c>
       <c r="D18" t="n">
-        <v>9</v>
-      </c>
-      <c r="E18" t="n">
-        <v>-0.21965074556432</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="E18" t="inlineStr"/>
       <c r="F18" t="n">
-        <v>0.3864499959296761</v>
+        <v>0.4921709386757383</v>
       </c>
       <c r="G18" t="n">
-        <v>0.8888888888888888</v>
+        <v>0.8730769230769231</v>
       </c>
       <c r="H18" t="n">
-        <v>0.6968434751923678</v>
+        <v>0.7338313652959783</v>
       </c>
       <c r="I18" t="n">
-        <v>0.9259782590668009</v>
+        <v>0.960014421531845</v>
       </c>
       <c r="J18" t="n">
-        <v>0.7350611883314511</v>
+        <v>0.7049224899422258</v>
       </c>
       <c r="K18" t="n">
-        <v>0.4373522458628842</v>
+        <v>0.1962174940898345</v>
       </c>
       <c r="L18" t="inlineStr">
         <is>
           <t>opt</t>
         </is>
       </c>
-      <c r="M18" t="n">
-        <v>-1.365618952536943</v>
-      </c>
+      <c r="M18" t="inlineStr"/>
       <c r="N18" t="n">
-        <v>0.1244115503594764</v>
+        <v>0.3989252683101294</v>
       </c>
     </row>
     <row r="19">
@@ -1388,32 +1384,32 @@
       </c>
       <c r="C19" t="inlineStr">
         <is>
-          <t>trial_14</t>
+          <t>trial_17</t>
         </is>
       </c>
       <c r="D19" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E19" t="n">
-        <v>-0.2064353951189201</v>
+        <v>-0.07854752183691655</v>
       </c>
       <c r="F19" t="n">
-        <v>0.4852884006919144</v>
+        <v>0.5586152558911119</v>
       </c>
       <c r="G19" t="n">
-        <v>0.92</v>
+        <v>0.8111111111111111</v>
       </c>
       <c r="H19" t="n">
-        <v>0.7760875846081373</v>
+        <v>0.675801840881281</v>
       </c>
       <c r="I19" t="n">
-        <v>0.9237000216296234</v>
+        <v>0.9136010313525275</v>
       </c>
       <c r="J19" t="n">
-        <v>0.702004565930465</v>
+        <v>0.6308247151964474</v>
       </c>
       <c r="K19" t="n">
-        <v>0.3120567375886525</v>
+        <v>0.2813238770685579</v>
       </c>
       <c r="L19" t="inlineStr">
         <is>
@@ -1421,10 +1417,10 @@
         </is>
       </c>
       <c r="M19" t="n">
-        <v>-0.7296251379162629</v>
+        <v>0.08300842034405694</v>
       </c>
       <c r="N19" t="n">
-        <v>0.475665773282284</v>
+        <v>-0.6149306241913908</v>
       </c>
     </row>
     <row r="20">
@@ -1440,39 +1436,43 @@
       </c>
       <c r="C20" t="inlineStr">
         <is>
-          <t>trial_15</t>
+          <t>trial_18</t>
         </is>
       </c>
       <c r="D20" t="n">
-        <v>26</v>
-      </c>
-      <c r="E20" t="inlineStr"/>
+        <v>11</v>
+      </c>
+      <c r="E20" t="n">
+        <v>-0.1033477241680074</v>
+      </c>
       <c r="F20" t="n">
-        <v>0.4921709386757383</v>
+        <v>0.5827991531288469</v>
       </c>
       <c r="G20" t="n">
-        <v>0.8730769230769231</v>
+        <v>0.7545454545454545</v>
       </c>
       <c r="H20" t="n">
-        <v>0.7338313652959783</v>
+        <v>0.7646837994693524</v>
       </c>
       <c r="I20" t="n">
-        <v>0.960014421531845</v>
+        <v>0.9336702159993365</v>
       </c>
       <c r="J20" t="n">
-        <v>0.7049224899422258</v>
+        <v>0.6245278498099541</v>
       </c>
       <c r="K20" t="n">
-        <v>0.1962174940898345</v>
+        <v>0.2198581560283688</v>
       </c>
       <c r="L20" t="inlineStr">
         <is>
           <t>opt</t>
         </is>
       </c>
-      <c r="M20" t="inlineStr"/>
+      <c r="M20" t="n">
+        <v>-0.1102804337088831</v>
+      </c>
       <c r="N20" t="n">
-        <v>0.3925758865252091</v>
+        <v>0.0962012080643771</v>
       </c>
     </row>
     <row r="21">
@@ -1488,43 +1488,39 @@
       </c>
       <c r="C21" t="inlineStr">
         <is>
-          <t>trial_17</t>
+          <t>trial_19</t>
         </is>
       </c>
       <c r="D21" t="n">
-        <v>9</v>
-      </c>
-      <c r="E21" t="n">
-        <v>-0.07854752183691655</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="E21" t="inlineStr"/>
       <c r="F21" t="n">
-        <v>0.5586152558911119</v>
+        <v>0.4743177008409302</v>
       </c>
       <c r="G21" t="n">
-        <v>0.8111111111111111</v>
+        <v>0.8869565217391304</v>
       </c>
       <c r="H21" t="n">
-        <v>0.675801840881281</v>
+        <v>0.7925182203726262</v>
       </c>
       <c r="I21" t="n">
-        <v>0.9136010313525275</v>
+        <v>0.933883762155545</v>
       </c>
       <c r="J21" t="n">
-        <v>0.6308247151964474</v>
+        <v>0.5731248908038505</v>
       </c>
       <c r="K21" t="n">
-        <v>0.2813238770685579</v>
+        <v>0.392434988179669</v>
       </c>
       <c r="L21" t="inlineStr">
         <is>
           <t>opt</t>
         </is>
       </c>
-      <c r="M21" t="n">
-        <v>0.1370986858940119</v>
-      </c>
+      <c r="M21" t="inlineStr"/>
       <c r="N21" t="n">
-        <v>-0.5127841834464235</v>
+        <v>0.05774821717716822</v>
       </c>
     </row>
     <row r="22">
@@ -1540,32 +1536,32 @@
       </c>
       <c r="C22" t="inlineStr">
         <is>
-          <t>trial_18</t>
+          <t>trial_22</t>
         </is>
       </c>
       <c r="D22" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E22" t="n">
-        <v>-0.1033477241680074</v>
+        <v>0.004858871438054922</v>
       </c>
       <c r="F22" t="n">
-        <v>0.5827991531288469</v>
+        <v>0.613064646925586</v>
       </c>
       <c r="G22" t="n">
-        <v>0.7545454545454545</v>
+        <v>0.7555555555555555</v>
       </c>
       <c r="H22" t="n">
-        <v>0.7646837994693524</v>
+        <v>0.7652688977203049</v>
       </c>
       <c r="I22" t="n">
-        <v>0.9336702159993365</v>
+        <v>0.9221909559551449</v>
       </c>
       <c r="J22" t="n">
-        <v>0.6245278498099541</v>
+        <v>0.6523579702388265</v>
       </c>
       <c r="K22" t="n">
-        <v>0.2198581560283688</v>
+        <v>0.3782505910165485</v>
       </c>
       <c r="L22" t="inlineStr">
         <is>
@@ -1573,10 +1569,10 @@
         </is>
       </c>
       <c r="M22" t="n">
-        <v>-0.05399867486320972</v>
+        <v>0.7129801881435667</v>
       </c>
       <c r="N22" t="n">
-        <v>0.1201386873450135</v>
+        <v>0.1616334731788907</v>
       </c>
     </row>
     <row r="23">
@@ -1592,39 +1588,43 @@
       </c>
       <c r="C23" t="inlineStr">
         <is>
-          <t>trial_19</t>
+          <t>trial_23</t>
         </is>
       </c>
       <c r="D23" t="n">
-        <v>23</v>
-      </c>
-      <c r="E23" t="inlineStr"/>
+        <v>12</v>
+      </c>
+      <c r="E23" t="n">
+        <v>-0.08745688522712085</v>
+      </c>
       <c r="F23" t="n">
-        <v>0.4743177008409302</v>
+        <v>0.5081010236768583</v>
       </c>
       <c r="G23" t="n">
-        <v>0.8869565217391304</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="H23" t="n">
-        <v>0.7925182203726262</v>
+        <v>0.771350049894783</v>
       </c>
       <c r="I23" t="n">
-        <v>0.933883762155545</v>
+        <v>0.9140186850203094</v>
       </c>
       <c r="J23" t="n">
-        <v>0.5731248908038505</v>
+        <v>0.5638788479717393</v>
       </c>
       <c r="K23" t="n">
-        <v>0.392434988179669</v>
+        <v>0.3286052009456265</v>
       </c>
       <c r="L23" t="inlineStr">
         <is>
           <t>opt</t>
         </is>
       </c>
-      <c r="M23" t="inlineStr"/>
+      <c r="M23" t="n">
+        <v>-0.1543978559193272</v>
+      </c>
       <c r="N23" t="n">
-        <v>0.07856821074145054</v>
+        <v>-0.247583991598846</v>
       </c>
     </row>
     <row r="24">
@@ -1640,32 +1640,32 @@
       </c>
       <c r="C24" t="inlineStr">
         <is>
-          <t>trial_22</t>
+          <t>trial_24</t>
         </is>
       </c>
       <c r="D24" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E24" t="n">
-        <v>0.004858871438054922</v>
+        <v>0.007560071814801735</v>
       </c>
       <c r="F24" t="n">
-        <v>0.613064646925586</v>
+        <v>0.6058599854512132</v>
       </c>
       <c r="G24" t="n">
-        <v>0.7555555555555555</v>
+        <v>0.75</v>
       </c>
       <c r="H24" t="n">
-        <v>0.7652688977203049</v>
+        <v>0.7895779214705489</v>
       </c>
       <c r="I24" t="n">
-        <v>0.9221909559551449</v>
+        <v>0.9262042731060053</v>
       </c>
       <c r="J24" t="n">
-        <v>0.6523579702388265</v>
+        <v>0.6036024422926879</v>
       </c>
       <c r="K24" t="n">
-        <v>0.3782505910165485</v>
+        <v>0.1442080378250591</v>
       </c>
       <c r="L24" t="inlineStr">
         <is>
@@ -1673,10 +1673,10 @@
         </is>
       </c>
       <c r="M24" t="n">
-        <v>0.7748401915162465</v>
+        <v>0.6800424648862116</v>
       </c>
       <c r="N24" t="n">
-        <v>0.1879826680823566</v>
+        <v>0.1323882490792015</v>
       </c>
     </row>
     <row r="25">
@@ -1692,32 +1692,32 @@
       </c>
       <c r="C25" t="inlineStr">
         <is>
-          <t>trial_23</t>
+          <t>trial_25</t>
         </is>
       </c>
       <c r="D25" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E25" t="n">
-        <v>-0.08745688522712085</v>
+        <v>-0.1854877594050874</v>
       </c>
       <c r="F25" t="n">
-        <v>0.5081010236768583</v>
+        <v>0.5511736541676847</v>
       </c>
       <c r="G25" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.8833333333333333</v>
       </c>
       <c r="H25" t="n">
-        <v>0.771350049894783</v>
+        <v>0.7988195699015044</v>
       </c>
       <c r="I25" t="n">
-        <v>0.9140186850203094</v>
+        <v>0.8928311850741076</v>
       </c>
       <c r="J25" t="n">
-        <v>0.5638788479717393</v>
+        <v>0.7534093282811004</v>
       </c>
       <c r="K25" t="n">
-        <v>0.3286052009456265</v>
+        <v>0.6264775413711584</v>
       </c>
       <c r="L25" t="inlineStr">
         <is>
@@ -1725,10 +1725,10 @@
         </is>
       </c>
       <c r="M25" t="n">
-        <v>-0.1005603264774428</v>
+        <v>-0.4224771234347467</v>
       </c>
       <c r="N25" t="n">
-        <v>-0.1897769893506367</v>
+        <v>0.690908395471777</v>
       </c>
     </row>
     <row r="26">
@@ -1744,43 +1744,39 @@
       </c>
       <c r="C26" t="inlineStr">
         <is>
-          <t>trial_24</t>
+          <t>trial_26</t>
         </is>
       </c>
       <c r="D26" t="n">
-        <v>12</v>
-      </c>
-      <c r="E26" t="n">
-        <v>0.007560071814801735</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="E26" t="inlineStr"/>
       <c r="F26" t="n">
-        <v>0.6058599854512132</v>
+        <v>0.556608677189084</v>
       </c>
       <c r="G26" t="n">
-        <v>0.75</v>
+        <v>0.8894736842105263</v>
       </c>
       <c r="H26" t="n">
-        <v>0.7895779214705489</v>
+        <v>0.7866868216016221</v>
       </c>
       <c r="I26" t="n">
-        <v>0.9262042731060053</v>
+        <v>0.9111523716635747</v>
       </c>
       <c r="J26" t="n">
-        <v>0.6036024422926879</v>
+        <v>0.5043857929568178</v>
       </c>
       <c r="K26" t="n">
-        <v>0.1442080378250591</v>
+        <v>0.3640661938534279</v>
       </c>
       <c r="L26" t="inlineStr">
         <is>
           <t>opt</t>
         </is>
       </c>
-      <c r="M26" t="n">
-        <v>0.7428743712302325</v>
-      </c>
+      <c r="M26" t="inlineStr"/>
       <c r="N26" t="n">
-        <v>0.153400003997961</v>
+        <v>-0.4285894000730903</v>
       </c>
     </row>
     <row r="27">
@@ -1796,32 +1792,32 @@
       </c>
       <c r="C27" t="inlineStr">
         <is>
-          <t>trial_25</t>
+          <t>trial_27</t>
         </is>
       </c>
       <c r="D27" t="n">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="E27" t="n">
-        <v>-0.1854877594050874</v>
+        <v>-0.1213273223639257</v>
       </c>
       <c r="F27" t="n">
-        <v>0.5511736541676847</v>
+        <v>0.5374958362529944</v>
       </c>
       <c r="G27" t="n">
-        <v>0.8833333333333333</v>
+        <v>0.90625</v>
       </c>
       <c r="H27" t="n">
-        <v>0.7988195699015044</v>
+        <v>0.7179601737158342</v>
       </c>
       <c r="I27" t="n">
-        <v>0.8928311850741076</v>
+        <v>0.9155986556322426</v>
       </c>
       <c r="J27" t="n">
-        <v>0.7534093282811004</v>
+        <v>0.633669422315583</v>
       </c>
       <c r="K27" t="n">
-        <v>0.6264775413711584</v>
+        <v>0.3806146572104019</v>
       </c>
       <c r="L27" t="inlineStr">
         <is>
@@ -1829,10 +1825,10 @@
         </is>
       </c>
       <c r="M27" t="n">
-        <v>-0.3811954416151656</v>
+        <v>-0.02516555646033342</v>
       </c>
       <c r="N27" t="n">
-        <v>0.692465672363468</v>
+        <v>-0.2942140010088521</v>
       </c>
     </row>
     <row r="28">
@@ -1848,39 +1844,43 @@
       </c>
       <c r="C28" t="inlineStr">
         <is>
-          <t>trial_26</t>
+          <t>trial_28</t>
         </is>
       </c>
       <c r="D28" t="n">
-        <v>19</v>
-      </c>
-      <c r="E28" t="inlineStr"/>
+        <v>16</v>
+      </c>
+      <c r="E28" t="n">
+        <v>-0.1213273223639257</v>
+      </c>
       <c r="F28" t="n">
-        <v>0.556608677189084</v>
+        <v>0.5374958362529944</v>
       </c>
       <c r="G28" t="n">
-        <v>0.8894736842105263</v>
+        <v>0.90625</v>
       </c>
       <c r="H28" t="n">
-        <v>0.7866868216016221</v>
+        <v>0.7179601737158342</v>
       </c>
       <c r="I28" t="n">
-        <v>0.9111523716635747</v>
+        <v>0.9155986556322426</v>
       </c>
       <c r="J28" t="n">
-        <v>0.5043857929568178</v>
+        <v>0.633669422315583</v>
       </c>
       <c r="K28" t="n">
-        <v>0.3640661938534279</v>
+        <v>0.3806146572104019</v>
       </c>
       <c r="L28" t="inlineStr">
         <is>
           <t>opt</t>
         </is>
       </c>
-      <c r="M28" t="inlineStr"/>
+      <c r="M28" t="n">
+        <v>-0.02516555646033342</v>
+      </c>
       <c r="N28" t="n">
-        <v>-0.3598631670728343</v>
+        <v>-0.2942140010088521</v>
       </c>
     </row>
     <row r="29">
@@ -1896,32 +1896,32 @@
       </c>
       <c r="C29" t="inlineStr">
         <is>
-          <t>trial_27</t>
+          <t>trial_30</t>
         </is>
       </c>
       <c r="D29" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E29" t="n">
-        <v>-0.1213273223639257</v>
+        <v>-0.03313921715550731</v>
       </c>
       <c r="F29" t="n">
-        <v>0.5374958362529944</v>
+        <v>0.5819872846140995</v>
       </c>
       <c r="G29" t="n">
-        <v>0.90625</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="H29" t="n">
-        <v>0.7179601737158342</v>
+        <v>0.7697393194884969</v>
       </c>
       <c r="I29" t="n">
-        <v>0.9155986556322426</v>
+        <v>0.929328096817758</v>
       </c>
       <c r="J29" t="n">
-        <v>0.633669422315583</v>
+        <v>0.6813184968077977</v>
       </c>
       <c r="K29" t="n">
-        <v>0.3806146572104019</v>
+        <v>0.4964539007092199</v>
       </c>
       <c r="L29" t="inlineStr">
         <is>
@@ -1929,10 +1929,10 @@
         </is>
       </c>
       <c r="M29" t="n">
-        <v>0.01890321421178193</v>
+        <v>0.5393434208800163</v>
       </c>
       <c r="N29" t="n">
-        <v>-0.2234780334192858</v>
+        <v>0.3666431476213039</v>
       </c>
     </row>
     <row r="30">
@@ -1948,32 +1948,32 @@
       </c>
       <c r="C30" t="inlineStr">
         <is>
-          <t>trial_28</t>
+          <t>trial_31</t>
         </is>
       </c>
       <c r="D30" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E30" t="n">
-        <v>-0.1213273223639257</v>
+        <v>0.01129193678825731</v>
       </c>
       <c r="F30" t="n">
-        <v>0.5374958362529944</v>
+        <v>0.6019632815671072</v>
       </c>
       <c r="G30" t="n">
-        <v>0.90625</v>
+        <v>0.7</v>
       </c>
       <c r="H30" t="n">
-        <v>0.7179601737158342</v>
+        <v>0.7622874507300536</v>
       </c>
       <c r="I30" t="n">
-        <v>0.9155986556322426</v>
+        <v>0.9303286225796836</v>
       </c>
       <c r="J30" t="n">
-        <v>0.633669422315583</v>
+        <v>0.6232665061001467</v>
       </c>
       <c r="K30" t="n">
-        <v>0.3806146572104019</v>
+        <v>0.2505910165484633</v>
       </c>
       <c r="L30" t="inlineStr">
         <is>
@@ -1981,10 +1981,10 @@
         </is>
       </c>
       <c r="M30" t="n">
-        <v>0.01890321421178193</v>
+        <v>0.5478810646321272</v>
       </c>
       <c r="N30" t="n">
-        <v>-0.2234780334192858</v>
+        <v>0.05436668472986758</v>
       </c>
     </row>
     <row r="31">
@@ -1995,37 +1995,37 @@
       </c>
       <c r="B31" t="inlineStr">
         <is>
-          <t>run_20250831T230602Z</t>
+          <t>run_20250831T231222Z</t>
         </is>
       </c>
       <c r="C31" t="inlineStr">
         <is>
-          <t>trial_30</t>
+          <t>trial_02</t>
         </is>
       </c>
       <c r="D31" t="n">
-        <v>9</v>
+        <v>5</v>
       </c>
       <c r="E31" t="n">
-        <v>-0.03313921715550731</v>
+        <v>-0.009294195170745088</v>
       </c>
       <c r="F31" t="n">
-        <v>0.5819872846140995</v>
+        <v>0.6704763233430437</v>
       </c>
       <c r="G31" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.88</v>
       </c>
       <c r="H31" t="n">
-        <v>0.7697393194884969</v>
+        <v>0.7966696047272578</v>
       </c>
       <c r="I31" t="n">
-        <v>0.929328096817758</v>
+        <v>0.6962349914880063</v>
       </c>
       <c r="J31" t="n">
-        <v>0.6813184968077977</v>
+        <v>0.6557866614047151</v>
       </c>
       <c r="K31" t="n">
-        <v>0.4964539007092199</v>
+        <v>0.3687943262411347</v>
       </c>
       <c r="L31" t="inlineStr">
         <is>
@@ -2033,10 +2033,10 @@
         </is>
       </c>
       <c r="M31" t="n">
-        <v>0.5934263175292882</v>
+        <v>1.240696200298959</v>
       </c>
       <c r="N31" t="n">
-        <v>0.3738765916234009</v>
+        <v>-0.9020462009769868</v>
       </c>
     </row>
     <row r="32">
@@ -2047,48 +2047,44 @@
       </c>
       <c r="B32" t="inlineStr">
         <is>
-          <t>run_20250831T230602Z</t>
+          <t>run_20250831T231222Z</t>
         </is>
       </c>
       <c r="C32" t="inlineStr">
         <is>
-          <t>trial_31</t>
+          <t>trial_03</t>
         </is>
       </c>
       <c r="D32" t="n">
-        <v>10</v>
-      </c>
-      <c r="E32" t="n">
-        <v>0.01129193678825731</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="E32" t="inlineStr"/>
       <c r="F32" t="n">
-        <v>0.6019632815671072</v>
+        <v>0.5026942135711703</v>
       </c>
       <c r="G32" t="n">
-        <v>0.7</v>
+        <v>0.89375</v>
       </c>
       <c r="H32" t="n">
-        <v>0.7622874507300536</v>
+        <v>0.7431078485521072</v>
       </c>
       <c r="I32" t="n">
-        <v>0.9303286225796836</v>
+        <v>0.9527068843159245</v>
       </c>
       <c r="J32" t="n">
-        <v>0.6232665061001467</v>
+        <v>0.6259126435805692</v>
       </c>
       <c r="K32" t="n">
-        <v>0.2505910165484633</v>
+        <v>0.2293144208037825</v>
       </c>
       <c r="L32" t="inlineStr">
         <is>
           <t>opt</t>
         </is>
       </c>
-      <c r="M32" t="n">
-        <v>0.6154297369146065</v>
-      </c>
+      <c r="M32" t="inlineStr"/>
       <c r="N32" t="n">
-        <v>0.08364651940419715</v>
+        <v>0.06046960019251917</v>
       </c>
     </row>
     <row r="33">
@@ -2104,43 +2100,39 @@
       </c>
       <c r="C33" t="inlineStr">
         <is>
-          <t>trial_02</t>
+          <t>trial_04</t>
         </is>
       </c>
       <c r="D33" t="n">
-        <v>5</v>
-      </c>
-      <c r="E33" t="n">
-        <v>-0.009294195170745088</v>
-      </c>
+        <v>32</v>
+      </c>
+      <c r="E33" t="inlineStr"/>
       <c r="F33" t="n">
-        <v>0.6704763233430437</v>
+        <v>0.5007400549962517</v>
       </c>
       <c r="G33" t="n">
-        <v>0.88</v>
+        <v>0.896875</v>
       </c>
       <c r="H33" t="n">
-        <v>0.7966696047272578</v>
+        <v>0.7407559591321291</v>
       </c>
       <c r="I33" t="n">
-        <v>0.6962349914880063</v>
+        <v>0.9527068843159245</v>
       </c>
       <c r="J33" t="n">
-        <v>0.6557866614047151</v>
+        <v>0.6259126435805692</v>
       </c>
       <c r="K33" t="n">
-        <v>0.3687943262411347</v>
+        <v>0.2293144208037825</v>
       </c>
       <c r="L33" t="inlineStr">
         <is>
           <t>opt</t>
         </is>
       </c>
-      <c r="M33" t="n">
-        <v>1.288389430540349</v>
-      </c>
+      <c r="M33" t="inlineStr"/>
       <c r="N33" t="n">
-        <v>-0.6729039221768882</v>
+        <v>0.04394520320549476</v>
       </c>
     </row>
     <row r="34">
@@ -2156,30 +2148,30 @@
       </c>
       <c r="C34" t="inlineStr">
         <is>
-          <t>trial_03</t>
+          <t>trial_06</t>
         </is>
       </c>
       <c r="D34" t="n">
-        <v>32</v>
+        <v>19</v>
       </c>
       <c r="E34" t="inlineStr"/>
       <c r="F34" t="n">
-        <v>0.5026942135711703</v>
+        <v>0.558908702247524</v>
       </c>
       <c r="G34" t="n">
-        <v>0.89375</v>
+        <v>0.7631578947368421</v>
       </c>
       <c r="H34" t="n">
-        <v>0.7431078485521072</v>
+        <v>0.7887656388684514</v>
       </c>
       <c r="I34" t="n">
-        <v>0.9527068843159245</v>
+        <v>0.9409809457188111</v>
       </c>
       <c r="J34" t="n">
-        <v>0.6259126435805692</v>
+        <v>0.6739024108489315</v>
       </c>
       <c r="K34" t="n">
-        <v>0.2293144208037825</v>
+        <v>0.1134751773049645</v>
       </c>
       <c r="L34" t="inlineStr">
         <is>
@@ -2188,7 +2180,7 @@
       </c>
       <c r="M34" t="inlineStr"/>
       <c r="N34" t="n">
-        <v>0.07961759065271459</v>
+        <v>0.5334247590051294</v>
       </c>
     </row>
     <row r="35">
@@ -2204,39 +2196,43 @@
       </c>
       <c r="C35" t="inlineStr">
         <is>
-          <t>trial_04</t>
+          <t>trial_08</t>
         </is>
       </c>
       <c r="D35" t="n">
-        <v>32</v>
-      </c>
-      <c r="E35" t="inlineStr"/>
+        <v>11</v>
+      </c>
+      <c r="E35" t="n">
+        <v>-0.1159830581436215</v>
+      </c>
       <c r="F35" t="n">
-        <v>0.5007400549962517</v>
+        <v>0.5095177213670161</v>
       </c>
       <c r="G35" t="n">
-        <v>0.896875</v>
+        <v>0.8636363636363636</v>
       </c>
       <c r="H35" t="n">
-        <v>0.7407559591321291</v>
+        <v>0.694816646831274</v>
       </c>
       <c r="I35" t="n">
-        <v>0.9527068843159245</v>
+        <v>0.9312312577930228</v>
       </c>
       <c r="J35" t="n">
-        <v>0.6259126435805692</v>
+        <v>0.7108990227773749</v>
       </c>
       <c r="K35" t="n">
-        <v>0.2293144208037825</v>
+        <v>0.3120567375886525</v>
       </c>
       <c r="L35" t="inlineStr">
         <is>
           <t>opt</t>
         </is>
       </c>
-      <c r="M35" t="inlineStr"/>
+      <c r="M35" t="n">
+        <v>-0.2427144336209154</v>
+      </c>
       <c r="N35" t="n">
-        <v>0.06468526252982804</v>
+        <v>-0.01343902643841988</v>
       </c>
     </row>
     <row r="36">
@@ -2252,39 +2248,43 @@
       </c>
       <c r="C36" t="inlineStr">
         <is>
-          <t>trial_06</t>
+          <t>trial_09</t>
         </is>
       </c>
       <c r="D36" t="n">
-        <v>19</v>
-      </c>
-      <c r="E36" t="inlineStr"/>
+        <v>10</v>
+      </c>
+      <c r="E36" t="n">
+        <v>-0.162764465091032</v>
+      </c>
       <c r="F36" t="n">
-        <v>0.558908702247524</v>
+        <v>0.4988097726646469</v>
       </c>
       <c r="G36" t="n">
-        <v>0.7631578947368421</v>
+        <v>0.86</v>
       </c>
       <c r="H36" t="n">
-        <v>0.7887656388684514</v>
+        <v>0.7959258737527763</v>
       </c>
       <c r="I36" t="n">
-        <v>0.9409809457188111</v>
+        <v>0.9235588126697172</v>
       </c>
       <c r="J36" t="n">
-        <v>0.6739024108489315</v>
+        <v>0.6468847649605362</v>
       </c>
       <c r="K36" t="n">
-        <v>0.1134751773049645</v>
+        <v>0.3073286052009456</v>
       </c>
       <c r="L36" t="inlineStr">
         <is>
           <t>opt</t>
         </is>
       </c>
-      <c r="M36" t="inlineStr"/>
+      <c r="M36" t="n">
+        <v>-0.5959736184458531</v>
+      </c>
       <c r="N36" t="n">
-        <v>0.5184686686776847</v>
+        <v>0.3598511507241394</v>
       </c>
     </row>
     <row r="37">
@@ -2300,32 +2300,32 @@
       </c>
       <c r="C37" t="inlineStr">
         <is>
-          <t>trial_08</t>
+          <t>trial_12</t>
         </is>
       </c>
       <c r="D37" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E37" t="n">
-        <v>-0.1159830581436215</v>
+        <v>-0.21965074556432</v>
       </c>
       <c r="F37" t="n">
-        <v>0.5095177213670161</v>
+        <v>0.3864499959296761</v>
       </c>
       <c r="G37" t="n">
-        <v>0.8636363636363636</v>
+        <v>0.8888888888888888</v>
       </c>
       <c r="H37" t="n">
-        <v>0.694816646831274</v>
+        <v>0.6968434751923678</v>
       </c>
       <c r="I37" t="n">
-        <v>0.9312312577930228</v>
+        <v>0.9259782590668009</v>
       </c>
       <c r="J37" t="n">
-        <v>0.7108990227773749</v>
+        <v>0.7350611883314511</v>
       </c>
       <c r="K37" t="n">
-        <v>0.3120567375886525</v>
+        <v>0.4373522458628842</v>
       </c>
       <c r="L37" t="inlineStr">
         <is>
@@ -2333,10 +2333,10 @@
         </is>
       </c>
       <c r="M37" t="n">
-        <v>-0.1933940189185419</v>
+        <v>-1.411503453159859</v>
       </c>
       <c r="N37" t="n">
-        <v>0.03344458991619226</v>
+        <v>0.08115795083589994</v>
       </c>
     </row>
     <row r="38">
@@ -2352,32 +2352,32 @@
       </c>
       <c r="C38" t="inlineStr">
         <is>
-          <t>trial_09</t>
+          <t>trial_14</t>
         </is>
       </c>
       <c r="D38" t="n">
         <v>10</v>
       </c>
       <c r="E38" t="n">
-        <v>-0.162764465091032</v>
+        <v>-0.2064353951189201</v>
       </c>
       <c r="F38" t="n">
-        <v>0.4988097726646469</v>
+        <v>0.4852884006919144</v>
       </c>
       <c r="G38" t="n">
-        <v>0.86</v>
+        <v>0.92</v>
       </c>
       <c r="H38" t="n">
-        <v>0.7959258737527763</v>
+        <v>0.7760875846081373</v>
       </c>
       <c r="I38" t="n">
-        <v>0.9235588126697172</v>
+        <v>0.9237000216296234</v>
       </c>
       <c r="J38" t="n">
-        <v>0.6468847649605362</v>
+        <v>0.702004565930465</v>
       </c>
       <c r="K38" t="n">
-        <v>0.3073286052009456</v>
+        <v>0.3120567375886525</v>
       </c>
       <c r="L38" t="inlineStr">
         <is>
@@ -2385,10 +2385,10 @@
         </is>
       </c>
       <c r="M38" t="n">
-        <v>-0.5488947546916891</v>
+        <v>-0.7693122561303717</v>
       </c>
       <c r="N38" t="n">
-        <v>0.3657818567694575</v>
+        <v>0.4735362393898789</v>
       </c>
     </row>
     <row r="39">
@@ -2404,43 +2404,39 @@
       </c>
       <c r="C39" t="inlineStr">
         <is>
-          <t>trial_12</t>
+          <t>trial_15</t>
         </is>
       </c>
       <c r="D39" t="n">
-        <v>9</v>
-      </c>
-      <c r="E39" t="n">
-        <v>-0.21965074556432</v>
-      </c>
+        <v>26</v>
+      </c>
+      <c r="E39" t="inlineStr"/>
       <c r="F39" t="n">
-        <v>0.3864499959296761</v>
+        <v>0.4921709386757383</v>
       </c>
       <c r="G39" t="n">
-        <v>0.8888888888888888</v>
+        <v>0.8730769230769231</v>
       </c>
       <c r="H39" t="n">
-        <v>0.6968434751923678</v>
+        <v>0.7338313652959783</v>
       </c>
       <c r="I39" t="n">
-        <v>0.9259782590668009</v>
+        <v>0.960014421531845</v>
       </c>
       <c r="J39" t="n">
-        <v>0.7350611883314511</v>
+        <v>0.7049224899422258</v>
       </c>
       <c r="K39" t="n">
-        <v>0.4373522458628842</v>
+        <v>0.1962174940898345</v>
       </c>
       <c r="L39" t="inlineStr">
         <is>
           <t>opt</t>
         </is>
       </c>
-      <c r="M39" t="n">
-        <v>-1.365618952536943</v>
-      </c>
+      <c r="M39" t="inlineStr"/>
       <c r="N39" t="n">
-        <v>0.1244115503594764</v>
+        <v>0.3989252683101294</v>
       </c>
     </row>
     <row r="40">
@@ -2456,32 +2452,32 @@
       </c>
       <c r="C40" t="inlineStr">
         <is>
-          <t>trial_14</t>
+          <t>trial_17</t>
         </is>
       </c>
       <c r="D40" t="n">
-        <v>10</v>
+        <v>9</v>
       </c>
       <c r="E40" t="n">
-        <v>-0.2064353951189201</v>
+        <v>-0.07854752183691655</v>
       </c>
       <c r="F40" t="n">
-        <v>0.4852884006919144</v>
+        <v>0.5586152558911119</v>
       </c>
       <c r="G40" t="n">
-        <v>0.92</v>
+        <v>0.8111111111111111</v>
       </c>
       <c r="H40" t="n">
-        <v>0.7760875846081373</v>
+        <v>0.675801840881281</v>
       </c>
       <c r="I40" t="n">
-        <v>0.9237000216296234</v>
+        <v>0.9136010313525275</v>
       </c>
       <c r="J40" t="n">
-        <v>0.702004565930465</v>
+        <v>0.6308247151964474</v>
       </c>
       <c r="K40" t="n">
-        <v>0.3120567375886525</v>
+        <v>0.2813238770685579</v>
       </c>
       <c r="L40" t="inlineStr">
         <is>
@@ -2489,10 +2485,10 @@
         </is>
       </c>
       <c r="M40" t="n">
-        <v>-0.7296251379162629</v>
+        <v>0.08300842034405694</v>
       </c>
       <c r="N40" t="n">
-        <v>0.475665773282284</v>
+        <v>-0.6149306241913908</v>
       </c>
     </row>
     <row r="41">
@@ -2508,39 +2504,43 @@
       </c>
       <c r="C41" t="inlineStr">
         <is>
-          <t>trial_15</t>
+          <t>trial_18</t>
         </is>
       </c>
       <c r="D41" t="n">
-        <v>26</v>
-      </c>
-      <c r="E41" t="inlineStr"/>
+        <v>11</v>
+      </c>
+      <c r="E41" t="n">
+        <v>-0.1033477241680074</v>
+      </c>
       <c r="F41" t="n">
-        <v>0.4921709386757383</v>
+        <v>0.5827991531288469</v>
       </c>
       <c r="G41" t="n">
-        <v>0.8730769230769231</v>
+        <v>0.7545454545454545</v>
       </c>
       <c r="H41" t="n">
-        <v>0.7338313652959783</v>
+        <v>0.7646837994693524</v>
       </c>
       <c r="I41" t="n">
-        <v>0.960014421531845</v>
+        <v>0.9336702159993365</v>
       </c>
       <c r="J41" t="n">
-        <v>0.7049224899422258</v>
+        <v>0.6245278498099541</v>
       </c>
       <c r="K41" t="n">
-        <v>0.1962174940898345</v>
+        <v>0.2198581560283688</v>
       </c>
       <c r="L41" t="inlineStr">
         <is>
           <t>opt</t>
         </is>
       </c>
-      <c r="M41" t="inlineStr"/>
+      <c r="M41" t="n">
+        <v>-0.1102804337088831</v>
+      </c>
       <c r="N41" t="n">
-        <v>0.3925758865252091</v>
+        <v>0.0962012080643771</v>
       </c>
     </row>
     <row r="42">
@@ -2556,43 +2556,39 @@
       </c>
       <c r="C42" t="inlineStr">
         <is>
-          <t>trial_17</t>
+          <t>trial_19</t>
         </is>
       </c>
       <c r="D42" t="n">
-        <v>9</v>
-      </c>
-      <c r="E42" t="n">
-        <v>-0.07854752183691655</v>
-      </c>
+        <v>23</v>
+      </c>
+      <c r="E42" t="inlineStr"/>
       <c r="F42" t="n">
-        <v>0.5586152558911119</v>
+        <v>0.4743177008409302</v>
       </c>
       <c r="G42" t="n">
-        <v>0.8111111111111111</v>
+        <v>0.8869565217391304</v>
       </c>
       <c r="H42" t="n">
-        <v>0.675801840881281</v>
+        <v>0.7925182203726262</v>
       </c>
       <c r="I42" t="n">
-        <v>0.9136010313525275</v>
+        <v>0.933883762155545</v>
       </c>
       <c r="J42" t="n">
-        <v>0.6308247151964474</v>
+        <v>0.5731248908038505</v>
       </c>
       <c r="K42" t="n">
-        <v>0.2813238770685579</v>
+        <v>0.392434988179669</v>
       </c>
       <c r="L42" t="inlineStr">
         <is>
           <t>opt</t>
         </is>
       </c>
-      <c r="M42" t="n">
-        <v>0.1370986858940119</v>
-      </c>
+      <c r="M42" t="inlineStr"/>
       <c r="N42" t="n">
-        <v>-0.5127841834464235</v>
+        <v>0.05774821717716822</v>
       </c>
     </row>
     <row r="43">
@@ -2608,32 +2604,32 @@
       </c>
       <c r="C43" t="inlineStr">
         <is>
-          <t>trial_18</t>
+          <t>trial_22</t>
         </is>
       </c>
       <c r="D43" t="n">
-        <v>11</v>
+        <v>9</v>
       </c>
       <c r="E43" t="n">
-        <v>-0.1033477241680074</v>
+        <v>0.004858871438054922</v>
       </c>
       <c r="F43" t="n">
-        <v>0.5827991531288469</v>
+        <v>0.613064646925586</v>
       </c>
       <c r="G43" t="n">
-        <v>0.7545454545454545</v>
+        <v>0.7555555555555555</v>
       </c>
       <c r="H43" t="n">
-        <v>0.7646837994693524</v>
+        <v>0.7652688977203049</v>
       </c>
       <c r="I43" t="n">
-        <v>0.9336702159993365</v>
+        <v>0.9221909559551449</v>
       </c>
       <c r="J43" t="n">
-        <v>0.6245278498099541</v>
+        <v>0.6523579702388265</v>
       </c>
       <c r="K43" t="n">
-        <v>0.2198581560283688</v>
+        <v>0.3782505910165485</v>
       </c>
       <c r="L43" t="inlineStr">
         <is>
@@ -2641,10 +2637,10 @@
         </is>
       </c>
       <c r="M43" t="n">
-        <v>-0.05399867486320972</v>
+        <v>0.7129801881435667</v>
       </c>
       <c r="N43" t="n">
-        <v>0.1201386873450135</v>
+        <v>0.1616334731788907</v>
       </c>
     </row>
     <row r="44">
@@ -2660,39 +2656,43 @@
       </c>
       <c r="C44" t="inlineStr">
         <is>
-          <t>trial_19</t>
+          <t>trial_23</t>
         </is>
       </c>
       <c r="D44" t="n">
-        <v>23</v>
-      </c>
-      <c r="E44" t="inlineStr"/>
+        <v>12</v>
+      </c>
+      <c r="E44" t="n">
+        <v>-0.08745688522712085</v>
+      </c>
       <c r="F44" t="n">
-        <v>0.4743177008409302</v>
+        <v>0.5081010236768583</v>
       </c>
       <c r="G44" t="n">
-        <v>0.8869565217391304</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="H44" t="n">
-        <v>0.7925182203726262</v>
+        <v>0.771350049894783</v>
       </c>
       <c r="I44" t="n">
-        <v>0.933883762155545</v>
+        <v>0.9140186850203094</v>
       </c>
       <c r="J44" t="n">
-        <v>0.5731248908038505</v>
+        <v>0.5638788479717393</v>
       </c>
       <c r="K44" t="n">
-        <v>0.392434988179669</v>
+        <v>0.3286052009456265</v>
       </c>
       <c r="L44" t="inlineStr">
         <is>
           <t>opt</t>
         </is>
       </c>
-      <c r="M44" t="inlineStr"/>
+      <c r="M44" t="n">
+        <v>-0.1543978559193272</v>
+      </c>
       <c r="N44" t="n">
-        <v>0.07856821074145054</v>
+        <v>-0.247583991598846</v>
       </c>
     </row>
     <row r="45">
@@ -2708,32 +2708,32 @@
       </c>
       <c r="C45" t="inlineStr">
         <is>
-          <t>trial_22</t>
+          <t>trial_24</t>
         </is>
       </c>
       <c r="D45" t="n">
-        <v>9</v>
+        <v>12</v>
       </c>
       <c r="E45" t="n">
-        <v>0.004858871438054922</v>
+        <v>0.007560071814801735</v>
       </c>
       <c r="F45" t="n">
-        <v>0.613064646925586</v>
+        <v>0.6058599854512132</v>
       </c>
       <c r="G45" t="n">
-        <v>0.7555555555555555</v>
+        <v>0.75</v>
       </c>
       <c r="H45" t="n">
-        <v>0.7652688977203049</v>
+        <v>0.7895779214705489</v>
       </c>
       <c r="I45" t="n">
-        <v>0.9221909559551449</v>
+        <v>0.9262042731060053</v>
       </c>
       <c r="J45" t="n">
-        <v>0.6523579702388265</v>
+        <v>0.6036024422926879</v>
       </c>
       <c r="K45" t="n">
-        <v>0.3782505910165485</v>
+        <v>0.1442080378250591</v>
       </c>
       <c r="L45" t="inlineStr">
         <is>
@@ -2741,10 +2741,10 @@
         </is>
       </c>
       <c r="M45" t="n">
-        <v>0.7748401915162465</v>
+        <v>0.6800424648862116</v>
       </c>
       <c r="N45" t="n">
-        <v>0.1879826680823566</v>
+        <v>0.1323882490792015</v>
       </c>
     </row>
     <row r="46">
@@ -2760,32 +2760,32 @@
       </c>
       <c r="C46" t="inlineStr">
         <is>
-          <t>trial_23</t>
+          <t>trial_25</t>
         </is>
       </c>
       <c r="D46" t="n">
-        <v>12</v>
+        <v>6</v>
       </c>
       <c r="E46" t="n">
-        <v>-0.08745688522712085</v>
+        <v>-0.1854877594050874</v>
       </c>
       <c r="F46" t="n">
-        <v>0.5081010236768583</v>
+        <v>0.5511736541676847</v>
       </c>
       <c r="G46" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.8833333333333333</v>
       </c>
       <c r="H46" t="n">
-        <v>0.771350049894783</v>
+        <v>0.7988195699015044</v>
       </c>
       <c r="I46" t="n">
-        <v>0.9140186850203094</v>
+        <v>0.8928311850741076</v>
       </c>
       <c r="J46" t="n">
-        <v>0.5638788479717393</v>
+        <v>0.7534093282811004</v>
       </c>
       <c r="K46" t="n">
-        <v>0.3286052009456265</v>
+        <v>0.6264775413711584</v>
       </c>
       <c r="L46" t="inlineStr">
         <is>
@@ -2793,10 +2793,10 @@
         </is>
       </c>
       <c r="M46" t="n">
-        <v>-0.1005603264774428</v>
+        <v>-0.4224771234347467</v>
       </c>
       <c r="N46" t="n">
-        <v>-0.1897769893506367</v>
+        <v>0.690908395471777</v>
       </c>
     </row>
     <row r="47">
@@ -2812,43 +2812,39 @@
       </c>
       <c r="C47" t="inlineStr">
         <is>
-          <t>trial_24</t>
+          <t>trial_26</t>
         </is>
       </c>
       <c r="D47" t="n">
-        <v>12</v>
-      </c>
-      <c r="E47" t="n">
-        <v>0.007560071814801735</v>
-      </c>
+        <v>19</v>
+      </c>
+      <c r="E47" t="inlineStr"/>
       <c r="F47" t="n">
-        <v>0.6058599854512132</v>
+        <v>0.556608677189084</v>
       </c>
       <c r="G47" t="n">
-        <v>0.75</v>
+        <v>0.8894736842105263</v>
       </c>
       <c r="H47" t="n">
-        <v>0.7895779214705489</v>
+        <v>0.7866868216016221</v>
       </c>
       <c r="I47" t="n">
-        <v>0.9262042731060053</v>
+        <v>0.9111523716635747</v>
       </c>
       <c r="J47" t="n">
-        <v>0.6036024422926879</v>
+        <v>0.5043857929568178</v>
       </c>
       <c r="K47" t="n">
-        <v>0.1442080378250591</v>
+        <v>0.3640661938534279</v>
       </c>
       <c r="L47" t="inlineStr">
         <is>
           <t>opt</t>
         </is>
       </c>
-      <c r="M47" t="n">
-        <v>0.7428743712302325</v>
-      </c>
+      <c r="M47" t="inlineStr"/>
       <c r="N47" t="n">
-        <v>0.153400003997961</v>
+        <v>-0.4285894000730903</v>
       </c>
     </row>
     <row r="48">
@@ -2864,32 +2860,32 @@
       </c>
       <c r="C48" t="inlineStr">
         <is>
-          <t>trial_25</t>
+          <t>trial_27</t>
         </is>
       </c>
       <c r="D48" t="n">
-        <v>6</v>
+        <v>16</v>
       </c>
       <c r="E48" t="n">
-        <v>-0.1854877594050874</v>
+        <v>-0.1213273223639257</v>
       </c>
       <c r="F48" t="n">
-        <v>0.5511736541676847</v>
+        <v>0.5374958362529944</v>
       </c>
       <c r="G48" t="n">
-        <v>0.8833333333333333</v>
+        <v>0.90625</v>
       </c>
       <c r="H48" t="n">
-        <v>0.7988195699015044</v>
+        <v>0.7179601737158342</v>
       </c>
       <c r="I48" t="n">
-        <v>0.8928311850741076</v>
+        <v>0.9155986556322426</v>
       </c>
       <c r="J48" t="n">
-        <v>0.7534093282811004</v>
+        <v>0.633669422315583</v>
       </c>
       <c r="K48" t="n">
-        <v>0.6264775413711584</v>
+        <v>0.3806146572104019</v>
       </c>
       <c r="L48" t="inlineStr">
         <is>
@@ -2897,10 +2893,10 @@
         </is>
       </c>
       <c r="M48" t="n">
-        <v>-0.3811954416151656</v>
+        <v>-0.02516555646033342</v>
       </c>
       <c r="N48" t="n">
-        <v>0.692465672363468</v>
+        <v>-0.2942140010088521</v>
       </c>
     </row>
     <row r="49">
@@ -2916,39 +2912,43 @@
       </c>
       <c r="C49" t="inlineStr">
         <is>
-          <t>trial_26</t>
+          <t>trial_28</t>
         </is>
       </c>
       <c r="D49" t="n">
-        <v>19</v>
-      </c>
-      <c r="E49" t="inlineStr"/>
+        <v>16</v>
+      </c>
+      <c r="E49" t="n">
+        <v>-0.1213273223639257</v>
+      </c>
       <c r="F49" t="n">
-        <v>0.556608677189084</v>
+        <v>0.5374958362529944</v>
       </c>
       <c r="G49" t="n">
-        <v>0.8894736842105263</v>
+        <v>0.90625</v>
       </c>
       <c r="H49" t="n">
-        <v>0.7866868216016221</v>
+        <v>0.7179601737158342</v>
       </c>
       <c r="I49" t="n">
-        <v>0.9111523716635747</v>
+        <v>0.9155986556322426</v>
       </c>
       <c r="J49" t="n">
-        <v>0.5043857929568178</v>
+        <v>0.633669422315583</v>
       </c>
       <c r="K49" t="n">
-        <v>0.3640661938534279</v>
+        <v>0.3806146572104019</v>
       </c>
       <c r="L49" t="inlineStr">
         <is>
           <t>opt</t>
         </is>
       </c>
-      <c r="M49" t="inlineStr"/>
+      <c r="M49" t="n">
+        <v>-0.02516555646033342</v>
+      </c>
       <c r="N49" t="n">
-        <v>-0.3598631670728343</v>
+        <v>-0.2942140010088521</v>
       </c>
     </row>
     <row r="50">
@@ -2964,32 +2964,32 @@
       </c>
       <c r="C50" t="inlineStr">
         <is>
-          <t>trial_27</t>
+          <t>trial_30</t>
         </is>
       </c>
       <c r="D50" t="n">
-        <v>16</v>
+        <v>9</v>
       </c>
       <c r="E50" t="n">
-        <v>-0.1213273223639257</v>
+        <v>-0.03313921715550731</v>
       </c>
       <c r="F50" t="n">
-        <v>0.5374958362529944</v>
+        <v>0.5819872846140995</v>
       </c>
       <c r="G50" t="n">
-        <v>0.90625</v>
+        <v>0.8333333333333334</v>
       </c>
       <c r="H50" t="n">
-        <v>0.7179601737158342</v>
+        <v>0.7697393194884969</v>
       </c>
       <c r="I50" t="n">
-        <v>0.9155986556322426</v>
+        <v>0.929328096817758</v>
       </c>
       <c r="J50" t="n">
-        <v>0.633669422315583</v>
+        <v>0.6813184968077977</v>
       </c>
       <c r="K50" t="n">
-        <v>0.3806146572104019</v>
+        <v>0.4964539007092199</v>
       </c>
       <c r="L50" t="inlineStr">
         <is>
@@ -2997,10 +2997,10 @@
         </is>
       </c>
       <c r="M50" t="n">
-        <v>0.01890321421178193</v>
+        <v>0.5393434208800163</v>
       </c>
       <c r="N50" t="n">
-        <v>-0.2234780334192858</v>
+        <v>0.3666431476213039</v>
       </c>
     </row>
     <row r="51">
@@ -3016,32 +3016,32 @@
       </c>
       <c r="C51" t="inlineStr">
         <is>
-          <t>trial_28</t>
+          <t>trial_31</t>
         </is>
       </c>
       <c r="D51" t="n">
-        <v>16</v>
+        <v>10</v>
       </c>
       <c r="E51" t="n">
-        <v>-0.1213273223639257</v>
+        <v>0.01129193678825731</v>
       </c>
       <c r="F51" t="n">
-        <v>0.5374958362529944</v>
+        <v>0.6019632815671072</v>
       </c>
       <c r="G51" t="n">
-        <v>0.90625</v>
+        <v>0.7</v>
       </c>
       <c r="H51" t="n">
-        <v>0.7179601737158342</v>
+        <v>0.7622874507300536</v>
       </c>
       <c r="I51" t="n">
-        <v>0.9155986556322426</v>
+        <v>0.9303286225796836</v>
       </c>
       <c r="J51" t="n">
-        <v>0.633669422315583</v>
+        <v>0.6232665061001467</v>
       </c>
       <c r="K51" t="n">
-        <v>0.3806146572104019</v>
+        <v>0.2505910165484633</v>
       </c>
       <c r="L51" t="inlineStr">
         <is>
@@ -3049,10 +3049,10 @@
         </is>
       </c>
       <c r="M51" t="n">
-        <v>0.01890321421178193</v>
+        <v>0.5478810646321272</v>
       </c>
       <c r="N51" t="n">
-        <v>-0.2234780334192858</v>
+        <v>0.05436668472986758</v>
       </c>
     </row>
     <row r="52">
@@ -3068,43 +3068,39 @@
       </c>
       <c r="C52" t="inlineStr">
         <is>
-          <t>trial_30</t>
+          <t>trial_32</t>
         </is>
       </c>
       <c r="D52" t="n">
-        <v>9</v>
-      </c>
-      <c r="E52" t="n">
-        <v>-0.03313921715550731</v>
-      </c>
+        <v>40</v>
+      </c>
+      <c r="E52" t="inlineStr"/>
       <c r="F52" t="n">
-        <v>0.5819872846140995</v>
+        <v>0.5844822845975053</v>
       </c>
       <c r="G52" t="n">
-        <v>0.8333333333333334</v>
+        <v>0.8825</v>
       </c>
       <c r="H52" t="n">
-        <v>0.7697393194884969</v>
+        <v>0.8111286869904576</v>
       </c>
       <c r="I52" t="n">
-        <v>0.929328096817758</v>
+        <v>0.9709287089865352</v>
       </c>
       <c r="J52" t="n">
-        <v>0.6813184968077977</v>
+        <v>0.6600227826517824</v>
       </c>
       <c r="K52" t="n">
-        <v>0.4964539007092199</v>
+        <v>0.2080378250591016</v>
       </c>
       <c r="L52" t="inlineStr">
         <is>
           <t>opt</t>
         </is>
       </c>
-      <c r="M52" t="n">
-        <v>0.5934263175292882</v>
-      </c>
+      <c r="M52" t="inlineStr"/>
       <c r="N52" t="n">
-        <v>0.3738765916234009</v>
+        <v>0.7993259091011755</v>
       </c>
     </row>
     <row r="53">
@@ -3120,43 +3116,39 @@
       </c>
       <c r="C53" t="inlineStr">
         <is>
-          <t>trial_31</t>
+          <t>trial_34</t>
         </is>
       </c>
       <c r="D53" t="n">
-        <v>10</v>
-      </c>
-      <c r="E53" t="n">
-        <v>0.01129193678825731</v>
-      </c>
+        <v>24</v>
+      </c>
+      <c r="E53" t="inlineStr"/>
       <c r="F53" t="n">
-        <v>0.6019632815671072</v>
+        <v>0.5402215860831115</v>
       </c>
       <c r="G53" t="n">
-        <v>0.7</v>
+        <v>0.8625</v>
       </c>
       <c r="H53" t="n">
-        <v>0.7622874507300536</v>
+        <v>0.8053422831043823</v>
       </c>
       <c r="I53" t="n">
-        <v>0.9303286225796836</v>
+        <v>0.9300197934529747</v>
       </c>
       <c r="J53" t="n">
-        <v>0.6232665061001467</v>
+        <v>0.5387192283327192</v>
       </c>
       <c r="K53" t="n">
-        <v>0.2505910165484633</v>
+        <v>0.3026004728132388</v>
       </c>
       <c r="L53" t="inlineStr">
         <is>
           <t>opt</t>
         </is>
       </c>
-      <c r="M53" t="n">
-        <v>0.6154297369146065</v>
-      </c>
+      <c r="M53" t="inlineStr"/>
       <c r="N53" t="n">
-        <v>0.08364651940419715</v>
+        <v>-0.03183845555468479</v>
       </c>
     </row>
     <row r="54">
@@ -3172,30 +3164,30 @@
       </c>
       <c r="C54" t="inlineStr">
         <is>
-          <t>trial_32</t>
+          <t>trial_35</t>
         </is>
       </c>
       <c r="D54" t="n">
-        <v>40</v>
+        <v>24</v>
       </c>
       <c r="E54" t="inlineStr"/>
       <c r="F54" t="n">
-        <v>0.5844822845975053</v>
+        <v>0.5694254587755775</v>
       </c>
       <c r="G54" t="n">
-        <v>0.8825</v>
+        <v>0.8666666666666667</v>
       </c>
       <c r="H54" t="n">
-        <v>0.8111286869904576</v>
+        <v>0.807645415680557</v>
       </c>
       <c r="I54" t="n">
-        <v>0.9709287089865352</v>
+        <v>0.923179492386858</v>
       </c>
       <c r="J54" t="n">
-        <v>0.6600227826517824</v>
+        <v>0.557086099435</v>
       </c>
       <c r="K54" t="n">
-        <v>0.2080378250591016</v>
+        <v>0.3333333333333333</v>
       </c>
       <c r="L54" t="inlineStr">
         <is>
@@ -3204,7 +3196,7 @@
       </c>
       <c r="M54" t="inlineStr"/>
       <c r="N54" t="n">
-        <v>0.7436989368043815</v>
+        <v>0.02904534839028916</v>
       </c>
     </row>
     <row r="55">
@@ -3220,39 +3212,43 @@
       </c>
       <c r="C55" t="inlineStr">
         <is>
-          <t>trial_34</t>
+          <t>trial_36</t>
         </is>
       </c>
       <c r="D55" t="n">
-        <v>24</v>
-      </c>
-      <c r="E55" t="inlineStr"/>
+        <v>17</v>
+      </c>
+      <c r="E55" t="n">
+        <v>-0.1890881146846022</v>
+      </c>
       <c r="F55" t="n">
-        <v>0.5402215860831115</v>
+        <v>0.4682691065008869</v>
       </c>
       <c r="G55" t="n">
-        <v>0.8625</v>
+        <v>0.8941176470588236</v>
       </c>
       <c r="H55" t="n">
-        <v>0.8053422831043823</v>
+        <v>0.7139096598127851</v>
       </c>
       <c r="I55" t="n">
-        <v>0.9300197934529747</v>
+        <v>0.9159061792619592</v>
       </c>
       <c r="J55" t="n">
-        <v>0.5387192283327192</v>
+        <v>0.5708918989924785</v>
       </c>
       <c r="K55" t="n">
-        <v>0.3026004728132388</v>
+        <v>0.2789598108747045</v>
       </c>
       <c r="L55" t="inlineStr">
         <is>
           <t>opt</t>
         </is>
       </c>
-      <c r="M55" t="inlineStr"/>
+      <c r="M55" t="n">
+        <v>-0.8135861474837538</v>
+      </c>
       <c r="N55" t="n">
-        <v>-0.00518260782005564</v>
+        <v>-0.6082060409174629</v>
       </c>
     </row>
     <row r="56">
@@ -3268,39 +3264,43 @@
       </c>
       <c r="C56" t="inlineStr">
         <is>
-          <t>trial_35</t>
+          <t>trial_39</t>
         </is>
       </c>
       <c r="D56" t="n">
-        <v>24</v>
-      </c>
-      <c r="E56" t="inlineStr"/>
+        <v>12</v>
+      </c>
+      <c r="E56" t="n">
+        <v>0.009048572224704156</v>
+      </c>
       <c r="F56" t="n">
-        <v>0.5694254587755775</v>
+        <v>0.5948303152692596</v>
       </c>
       <c r="G56" t="n">
-        <v>0.8666666666666667</v>
+        <v>0.7083333333333334</v>
       </c>
       <c r="H56" t="n">
-        <v>0.807645415680557</v>
+        <v>0.7916744452506473</v>
       </c>
       <c r="I56" t="n">
-        <v>0.923179492386858</v>
+        <v>0.9228149007779421</v>
       </c>
       <c r="J56" t="n">
-        <v>0.557086099435</v>
+        <v>0.6453452726951627</v>
       </c>
       <c r="K56" t="n">
-        <v>0.3333333333333333</v>
+        <v>0.2340425531914894</v>
       </c>
       <c r="L56" t="inlineStr">
         <is>
           <t>opt</t>
         </is>
       </c>
-      <c r="M56" t="inlineStr"/>
+      <c r="M56" t="n">
+        <v>0.5224175118152086</v>
+      </c>
       <c r="N56" t="n">
-        <v>0.05526232216749682</v>
+        <v>0.3186551133520608</v>
       </c>
     </row>
     <row r="57">
@@ -3311,37 +3311,37 @@
       </c>
       <c r="B57" t="inlineStr">
         <is>
-          <t>run_20250831T231222Z</t>
+          <t>run_20250901T165942Z</t>
         </is>
       </c>
       <c r="C57" t="inlineStr">
         <is>
-          <t>trial_36</t>
+          <t>trial_02</t>
         </is>
       </c>
       <c r="D57" t="n">
-        <v>17</v>
+        <v>6</v>
       </c>
       <c r="E57" t="n">
-        <v>-0.1890881146846022</v>
+        <v>-0.1036481696278762</v>
       </c>
       <c r="F57" t="n">
-        <v>0.4682691065008869</v>
+        <v>0.6505978159772585</v>
       </c>
       <c r="G57" t="n">
-        <v>0.8941176470588236</v>
+        <v>0.9166666666666666</v>
       </c>
       <c r="H57" t="n">
-        <v>0.7139096598127851</v>
+        <v>0.7964118694248346</v>
       </c>
       <c r="I57" t="n">
-        <v>0.9159061792619592</v>
+        <v>0.8359601236154192</v>
       </c>
       <c r="J57" t="n">
-        <v>0.5708918989924785</v>
+        <v>0.6491606370470357</v>
       </c>
       <c r="K57" t="n">
-        <v>0.2789598108747045</v>
+        <v>0.5011820330969267</v>
       </c>
       <c r="L57" t="inlineStr">
         <is>
@@ -3349,10 +3349,10 @@
         </is>
       </c>
       <c r="M57" t="n">
-        <v>-0.7697952780780888</v>
+        <v>0.6567837702910052</v>
       </c>
       <c r="N57" t="n">
-        <v>-0.5155706222251626</v>
+        <v>-0.1303003447728534</v>
       </c>
     </row>
     <row r="58">
@@ -3363,48 +3363,1212 @@
       </c>
       <c r="B58" t="inlineStr">
         <is>
-          <t>run_20250831T231222Z</t>
+          <t>run_20250901T165942Z</t>
         </is>
       </c>
       <c r="C58" t="inlineStr">
         <is>
+          <t>trial_03</t>
+        </is>
+      </c>
+      <c r="D58" t="n">
+        <v>32</v>
+      </c>
+      <c r="E58" t="inlineStr"/>
+      <c r="F58" t="n">
+        <v>0.5026942135711703</v>
+      </c>
+      <c r="G58" t="n">
+        <v>0.89375</v>
+      </c>
+      <c r="H58" t="n">
+        <v>0.7431078485521072</v>
+      </c>
+      <c r="I58" t="n">
+        <v>0.9527068843159245</v>
+      </c>
+      <c r="J58" t="n">
+        <v>0.6259126435805692</v>
+      </c>
+      <c r="K58" t="n">
+        <v>0.2293144208037825</v>
+      </c>
+      <c r="L58" t="inlineStr">
+        <is>
+          <t>opt</t>
+        </is>
+      </c>
+      <c r="M58" t="inlineStr"/>
+      <c r="N58" t="n">
+        <v>0.06046960019251917</v>
+      </c>
+    </row>
+    <row r="59">
+      <c r="A59" t="inlineStr">
+        <is>
+          <t>bertopic</t>
+        </is>
+      </c>
+      <c r="B59" t="inlineStr">
+        <is>
+          <t>run_20250901T165942Z</t>
+        </is>
+      </c>
+      <c r="C59" t="inlineStr">
+        <is>
+          <t>trial_04</t>
+        </is>
+      </c>
+      <c r="D59" t="n">
+        <v>32</v>
+      </c>
+      <c r="E59" t="inlineStr"/>
+      <c r="F59" t="n">
+        <v>0.5007400549962517</v>
+      </c>
+      <c r="G59" t="n">
+        <v>0.896875</v>
+      </c>
+      <c r="H59" t="n">
+        <v>0.7407559591321291</v>
+      </c>
+      <c r="I59" t="n">
+        <v>0.9527068843159245</v>
+      </c>
+      <c r="J59" t="n">
+        <v>0.6259126435805692</v>
+      </c>
+      <c r="K59" t="n">
+        <v>0.2293144208037825</v>
+      </c>
+      <c r="L59" t="inlineStr">
+        <is>
+          <t>opt</t>
+        </is>
+      </c>
+      <c r="M59" t="inlineStr"/>
+      <c r="N59" t="n">
+        <v>0.04394520320549476</v>
+      </c>
+    </row>
+    <row r="60">
+      <c r="A60" t="inlineStr">
+        <is>
+          <t>bertopic</t>
+        </is>
+      </c>
+      <c r="B60" t="inlineStr">
+        <is>
+          <t>run_20250901T165942Z</t>
+        </is>
+      </c>
+      <c r="C60" t="inlineStr">
+        <is>
+          <t>trial_06</t>
+        </is>
+      </c>
+      <c r="D60" t="n">
+        <v>19</v>
+      </c>
+      <c r="E60" t="inlineStr"/>
+      <c r="F60" t="n">
+        <v>0.558908702247524</v>
+      </c>
+      <c r="G60" t="n">
+        <v>0.7631578947368421</v>
+      </c>
+      <c r="H60" t="n">
+        <v>0.7887656388684514</v>
+      </c>
+      <c r="I60" t="n">
+        <v>0.9409809457188111</v>
+      </c>
+      <c r="J60" t="n">
+        <v>0.6739024108489315</v>
+      </c>
+      <c r="K60" t="n">
+        <v>0.1134751773049645</v>
+      </c>
+      <c r="L60" t="inlineStr">
+        <is>
+          <t>opt</t>
+        </is>
+      </c>
+      <c r="M60" t="inlineStr"/>
+      <c r="N60" t="n">
+        <v>0.5334247590051294</v>
+      </c>
+    </row>
+    <row r="61">
+      <c r="A61" t="inlineStr">
+        <is>
+          <t>bertopic</t>
+        </is>
+      </c>
+      <c r="B61" t="inlineStr">
+        <is>
+          <t>run_20250901T165942Z</t>
+        </is>
+      </c>
+      <c r="C61" t="inlineStr">
+        <is>
+          <t>trial_08</t>
+        </is>
+      </c>
+      <c r="D61" t="n">
+        <v>10</v>
+      </c>
+      <c r="E61" t="n">
+        <v>-0.1269186739747705</v>
+      </c>
+      <c r="F61" t="n">
+        <v>0.430632870018162</v>
+      </c>
+      <c r="G61" t="n">
+        <v>0.9</v>
+      </c>
+      <c r="H61" t="n">
+        <v>0.6918583364919813</v>
+      </c>
+      <c r="I61" t="n">
+        <v>0.8905002772962636</v>
+      </c>
+      <c r="J61" t="n">
+        <v>0.6910758251167218</v>
+      </c>
+      <c r="K61" t="n">
+        <v>0.2340425531914894</v>
+      </c>
+      <c r="L61" t="inlineStr">
+        <is>
+          <t>opt</t>
+        </is>
+      </c>
+      <c r="M61" t="n">
+        <v>-0.590336971284246</v>
+      </c>
+      <c r="N61" t="n">
+        <v>-0.3592829448266834</v>
+      </c>
+    </row>
+    <row r="62">
+      <c r="A62" t="inlineStr">
+        <is>
+          <t>bertopic</t>
+        </is>
+      </c>
+      <c r="B62" t="inlineStr">
+        <is>
+          <t>run_20250901T165942Z</t>
+        </is>
+      </c>
+      <c r="C62" t="inlineStr">
+        <is>
+          <t>trial_09</t>
+        </is>
+      </c>
+      <c r="D62" t="n">
+        <v>10</v>
+      </c>
+      <c r="E62" t="n">
+        <v>-0.1444746520885362</v>
+      </c>
+      <c r="F62" t="n">
+        <v>0.4992851754818227</v>
+      </c>
+      <c r="G62" t="n">
+        <v>0.88</v>
+      </c>
+      <c r="H62" t="n">
+        <v>0.7960405662499628</v>
+      </c>
+      <c r="I62" t="n">
+        <v>0.9274753131381483</v>
+      </c>
+      <c r="J62" t="n">
+        <v>0.681657115384679</v>
+      </c>
+      <c r="K62" t="n">
+        <v>0.293144208037825</v>
+      </c>
+      <c r="L62" t="inlineStr">
+        <is>
+          <t>opt</t>
+        </is>
+      </c>
+      <c r="M62" t="n">
+        <v>-0.4248784249228251</v>
+      </c>
+      <c r="N62" t="n">
+        <v>0.5423260228329674</v>
+      </c>
+    </row>
+    <row r="63">
+      <c r="A63" t="inlineStr">
+        <is>
+          <t>bertopic</t>
+        </is>
+      </c>
+      <c r="B63" t="inlineStr">
+        <is>
+          <t>run_20250901T165942Z</t>
+        </is>
+      </c>
+      <c r="C63" t="inlineStr">
+        <is>
+          <t>trial_12</t>
+        </is>
+      </c>
+      <c r="D63" t="n">
+        <v>9</v>
+      </c>
+      <c r="E63" t="n">
+        <v>-0.21965074556432</v>
+      </c>
+      <c r="F63" t="n">
+        <v>0.3864499959296761</v>
+      </c>
+      <c r="G63" t="n">
+        <v>0.8888888888888888</v>
+      </c>
+      <c r="H63" t="n">
+        <v>0.6968434751923678</v>
+      </c>
+      <c r="I63" t="n">
+        <v>0.9259782590668009</v>
+      </c>
+      <c r="J63" t="n">
+        <v>0.7350611883314511</v>
+      </c>
+      <c r="K63" t="n">
+        <v>0.4373522458628842</v>
+      </c>
+      <c r="L63" t="inlineStr">
+        <is>
+          <t>opt</t>
+        </is>
+      </c>
+      <c r="M63" t="n">
+        <v>-1.411503453159859</v>
+      </c>
+      <c r="N63" t="n">
+        <v>0.08115795083589994</v>
+      </c>
+    </row>
+    <row r="64">
+      <c r="A64" t="inlineStr">
+        <is>
+          <t>bertopic</t>
+        </is>
+      </c>
+      <c r="B64" t="inlineStr">
+        <is>
+          <t>run_20250901T165942Z</t>
+        </is>
+      </c>
+      <c r="C64" t="inlineStr">
+        <is>
+          <t>trial_14</t>
+        </is>
+      </c>
+      <c r="D64" t="n">
+        <v>10</v>
+      </c>
+      <c r="E64" t="n">
+        <v>-0.2064353951189201</v>
+      </c>
+      <c r="F64" t="n">
+        <v>0.4852884006919144</v>
+      </c>
+      <c r="G64" t="n">
+        <v>0.92</v>
+      </c>
+      <c r="H64" t="n">
+        <v>0.7760875846081373</v>
+      </c>
+      <c r="I64" t="n">
+        <v>0.9237000216296234</v>
+      </c>
+      <c r="J64" t="n">
+        <v>0.702004565930465</v>
+      </c>
+      <c r="K64" t="n">
+        <v>0.3120567375886525</v>
+      </c>
+      <c r="L64" t="inlineStr">
+        <is>
+          <t>opt</t>
+        </is>
+      </c>
+      <c r="M64" t="n">
+        <v>-0.7693122561303717</v>
+      </c>
+      <c r="N64" t="n">
+        <v>0.4735362393898789</v>
+      </c>
+    </row>
+    <row r="65">
+      <c r="A65" t="inlineStr">
+        <is>
+          <t>bertopic</t>
+        </is>
+      </c>
+      <c r="B65" t="inlineStr">
+        <is>
+          <t>run_20250901T165942Z</t>
+        </is>
+      </c>
+      <c r="C65" t="inlineStr">
+        <is>
+          <t>trial_15</t>
+        </is>
+      </c>
+      <c r="D65" t="n">
+        <v>26</v>
+      </c>
+      <c r="E65" t="inlineStr"/>
+      <c r="F65" t="n">
+        <v>0.4921709386757383</v>
+      </c>
+      <c r="G65" t="n">
+        <v>0.8730769230769231</v>
+      </c>
+      <c r="H65" t="n">
+        <v>0.7338313652959783</v>
+      </c>
+      <c r="I65" t="n">
+        <v>0.960014421531845</v>
+      </c>
+      <c r="J65" t="n">
+        <v>0.7049224899422258</v>
+      </c>
+      <c r="K65" t="n">
+        <v>0.1962174940898345</v>
+      </c>
+      <c r="L65" t="inlineStr">
+        <is>
+          <t>opt</t>
+        </is>
+      </c>
+      <c r="M65" t="inlineStr"/>
+      <c r="N65" t="n">
+        <v>0.3989252683101294</v>
+      </c>
+    </row>
+    <row r="66">
+      <c r="A66" t="inlineStr">
+        <is>
+          <t>bertopic</t>
+        </is>
+      </c>
+      <c r="B66" t="inlineStr">
+        <is>
+          <t>run_20250901T165942Z</t>
+        </is>
+      </c>
+      <c r="C66" t="inlineStr">
+        <is>
+          <t>trial_17</t>
+        </is>
+      </c>
+      <c r="D66" t="n">
+        <v>9</v>
+      </c>
+      <c r="E66" t="n">
+        <v>-0.07854752183691655</v>
+      </c>
+      <c r="F66" t="n">
+        <v>0.5586152558911119</v>
+      </c>
+      <c r="G66" t="n">
+        <v>0.8111111111111111</v>
+      </c>
+      <c r="H66" t="n">
+        <v>0.675801840881281</v>
+      </c>
+      <c r="I66" t="n">
+        <v>0.9136010313525275</v>
+      </c>
+      <c r="J66" t="n">
+        <v>0.6308247151964474</v>
+      </c>
+      <c r="K66" t="n">
+        <v>0.2813238770685579</v>
+      </c>
+      <c r="L66" t="inlineStr">
+        <is>
+          <t>opt</t>
+        </is>
+      </c>
+      <c r="M66" t="n">
+        <v>0.08300842034405694</v>
+      </c>
+      <c r="N66" t="n">
+        <v>-0.6149306241913908</v>
+      </c>
+    </row>
+    <row r="67">
+      <c r="A67" t="inlineStr">
+        <is>
+          <t>bertopic</t>
+        </is>
+      </c>
+      <c r="B67" t="inlineStr">
+        <is>
+          <t>run_20250901T165942Z</t>
+        </is>
+      </c>
+      <c r="C67" t="inlineStr">
+        <is>
+          <t>trial_18</t>
+        </is>
+      </c>
+      <c r="D67" t="n">
+        <v>11</v>
+      </c>
+      <c r="E67" t="n">
+        <v>-0.1033477241680074</v>
+      </c>
+      <c r="F67" t="n">
+        <v>0.5827991531288469</v>
+      </c>
+      <c r="G67" t="n">
+        <v>0.7545454545454545</v>
+      </c>
+      <c r="H67" t="n">
+        <v>0.7646837994693524</v>
+      </c>
+      <c r="I67" t="n">
+        <v>0.9336702159993365</v>
+      </c>
+      <c r="J67" t="n">
+        <v>0.6245278498099541</v>
+      </c>
+      <c r="K67" t="n">
+        <v>0.2198581560283688</v>
+      </c>
+      <c r="L67" t="inlineStr">
+        <is>
+          <t>opt</t>
+        </is>
+      </c>
+      <c r="M67" t="n">
+        <v>-0.1102804337088831</v>
+      </c>
+      <c r="N67" t="n">
+        <v>0.0962012080643771</v>
+      </c>
+    </row>
+    <row r="68">
+      <c r="A68" t="inlineStr">
+        <is>
+          <t>bertopic</t>
+        </is>
+      </c>
+      <c r="B68" t="inlineStr">
+        <is>
+          <t>run_20250901T165942Z</t>
+        </is>
+      </c>
+      <c r="C68" t="inlineStr">
+        <is>
+          <t>trial_19</t>
+        </is>
+      </c>
+      <c r="D68" t="n">
+        <v>23</v>
+      </c>
+      <c r="E68" t="inlineStr"/>
+      <c r="F68" t="n">
+        <v>0.4743177008409302</v>
+      </c>
+      <c r="G68" t="n">
+        <v>0.8869565217391304</v>
+      </c>
+      <c r="H68" t="n">
+        <v>0.7925182203726262</v>
+      </c>
+      <c r="I68" t="n">
+        <v>0.933883762155545</v>
+      </c>
+      <c r="J68" t="n">
+        <v>0.5731248908038505</v>
+      </c>
+      <c r="K68" t="n">
+        <v>0.392434988179669</v>
+      </c>
+      <c r="L68" t="inlineStr">
+        <is>
+          <t>opt</t>
+        </is>
+      </c>
+      <c r="M68" t="inlineStr"/>
+      <c r="N68" t="n">
+        <v>0.05774821717716822</v>
+      </c>
+    </row>
+    <row r="69">
+      <c r="A69" t="inlineStr">
+        <is>
+          <t>bertopic</t>
+        </is>
+      </c>
+      <c r="B69" t="inlineStr">
+        <is>
+          <t>run_20250901T165942Z</t>
+        </is>
+      </c>
+      <c r="C69" t="inlineStr">
+        <is>
+          <t>trial_22</t>
+        </is>
+      </c>
+      <c r="D69" t="n">
+        <v>9</v>
+      </c>
+      <c r="E69" t="n">
+        <v>0.004858871438054922</v>
+      </c>
+      <c r="F69" t="n">
+        <v>0.613064646925586</v>
+      </c>
+      <c r="G69" t="n">
+        <v>0.7555555555555555</v>
+      </c>
+      <c r="H69" t="n">
+        <v>0.7652688977203049</v>
+      </c>
+      <c r="I69" t="n">
+        <v>0.9221909559551449</v>
+      </c>
+      <c r="J69" t="n">
+        <v>0.6523579702388265</v>
+      </c>
+      <c r="K69" t="n">
+        <v>0.3782505910165485</v>
+      </c>
+      <c r="L69" t="inlineStr">
+        <is>
+          <t>opt</t>
+        </is>
+      </c>
+      <c r="M69" t="n">
+        <v>0.7129801881435667</v>
+      </c>
+      <c r="N69" t="n">
+        <v>0.1616334731788907</v>
+      </c>
+    </row>
+    <row r="70">
+      <c r="A70" t="inlineStr">
+        <is>
+          <t>bertopic</t>
+        </is>
+      </c>
+      <c r="B70" t="inlineStr">
+        <is>
+          <t>run_20250901T165942Z</t>
+        </is>
+      </c>
+      <c r="C70" t="inlineStr">
+        <is>
+          <t>trial_23</t>
+        </is>
+      </c>
+      <c r="D70" t="n">
+        <v>12</v>
+      </c>
+      <c r="E70" t="n">
+        <v>-0.08745688522712085</v>
+      </c>
+      <c r="F70" t="n">
+        <v>0.5081010236768583</v>
+      </c>
+      <c r="G70" t="n">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="H70" t="n">
+        <v>0.771350049894783</v>
+      </c>
+      <c r="I70" t="n">
+        <v>0.9140186850203094</v>
+      </c>
+      <c r="J70" t="n">
+        <v>0.5638788479717393</v>
+      </c>
+      <c r="K70" t="n">
+        <v>0.3286052009456265</v>
+      </c>
+      <c r="L70" t="inlineStr">
+        <is>
+          <t>opt</t>
+        </is>
+      </c>
+      <c r="M70" t="n">
+        <v>-0.1543978559193272</v>
+      </c>
+      <c r="N70" t="n">
+        <v>-0.247583991598846</v>
+      </c>
+    </row>
+    <row r="71">
+      <c r="A71" t="inlineStr">
+        <is>
+          <t>bertopic</t>
+        </is>
+      </c>
+      <c r="B71" t="inlineStr">
+        <is>
+          <t>run_20250901T165942Z</t>
+        </is>
+      </c>
+      <c r="C71" t="inlineStr">
+        <is>
+          <t>trial_24</t>
+        </is>
+      </c>
+      <c r="D71" t="n">
+        <v>12</v>
+      </c>
+      <c r="E71" t="n">
+        <v>0.007560071814801735</v>
+      </c>
+      <c r="F71" t="n">
+        <v>0.6058599854512132</v>
+      </c>
+      <c r="G71" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="H71" t="n">
+        <v>0.7895779214705489</v>
+      </c>
+      <c r="I71" t="n">
+        <v>0.9262042731060053</v>
+      </c>
+      <c r="J71" t="n">
+        <v>0.6036024422926879</v>
+      </c>
+      <c r="K71" t="n">
+        <v>0.1442080378250591</v>
+      </c>
+      <c r="L71" t="inlineStr">
+        <is>
+          <t>opt</t>
+        </is>
+      </c>
+      <c r="M71" t="n">
+        <v>0.6800424648862116</v>
+      </c>
+      <c r="N71" t="n">
+        <v>0.1323882490792015</v>
+      </c>
+    </row>
+    <row r="72">
+      <c r="A72" t="inlineStr">
+        <is>
+          <t>bertopic</t>
+        </is>
+      </c>
+      <c r="B72" t="inlineStr">
+        <is>
+          <t>run_20250901T165942Z</t>
+        </is>
+      </c>
+      <c r="C72" t="inlineStr">
+        <is>
+          <t>trial_25</t>
+        </is>
+      </c>
+      <c r="D72" t="n">
+        <v>6</v>
+      </c>
+      <c r="E72" t="n">
+        <v>-0.1854877594050874</v>
+      </c>
+      <c r="F72" t="n">
+        <v>0.5511736541676847</v>
+      </c>
+      <c r="G72" t="n">
+        <v>0.8833333333333333</v>
+      </c>
+      <c r="H72" t="n">
+        <v>0.7988195699015044</v>
+      </c>
+      <c r="I72" t="n">
+        <v>0.8928311850741076</v>
+      </c>
+      <c r="J72" t="n">
+        <v>0.7534093282811004</v>
+      </c>
+      <c r="K72" t="n">
+        <v>0.6264775413711584</v>
+      </c>
+      <c r="L72" t="inlineStr">
+        <is>
+          <t>opt</t>
+        </is>
+      </c>
+      <c r="M72" t="n">
+        <v>-0.4224771234347467</v>
+      </c>
+      <c r="N72" t="n">
+        <v>0.690908395471777</v>
+      </c>
+    </row>
+    <row r="73">
+      <c r="A73" t="inlineStr">
+        <is>
+          <t>bertopic</t>
+        </is>
+      </c>
+      <c r="B73" t="inlineStr">
+        <is>
+          <t>run_20250901T165942Z</t>
+        </is>
+      </c>
+      <c r="C73" t="inlineStr">
+        <is>
+          <t>trial_26</t>
+        </is>
+      </c>
+      <c r="D73" t="n">
+        <v>19</v>
+      </c>
+      <c r="E73" t="inlineStr"/>
+      <c r="F73" t="n">
+        <v>0.556608677189084</v>
+      </c>
+      <c r="G73" t="n">
+        <v>0.8894736842105263</v>
+      </c>
+      <c r="H73" t="n">
+        <v>0.7866868216016221</v>
+      </c>
+      <c r="I73" t="n">
+        <v>0.9111523716635747</v>
+      </c>
+      <c r="J73" t="n">
+        <v>0.5043857929568178</v>
+      </c>
+      <c r="K73" t="n">
+        <v>0.3640661938534279</v>
+      </c>
+      <c r="L73" t="inlineStr">
+        <is>
+          <t>opt</t>
+        </is>
+      </c>
+      <c r="M73" t="inlineStr"/>
+      <c r="N73" t="n">
+        <v>-0.4285894000730903</v>
+      </c>
+    </row>
+    <row r="74">
+      <c r="A74" t="inlineStr">
+        <is>
+          <t>bertopic</t>
+        </is>
+      </c>
+      <c r="B74" t="inlineStr">
+        <is>
+          <t>run_20250901T165942Z</t>
+        </is>
+      </c>
+      <c r="C74" t="inlineStr">
+        <is>
+          <t>trial_27</t>
+        </is>
+      </c>
+      <c r="D74" t="n">
+        <v>16</v>
+      </c>
+      <c r="E74" t="n">
+        <v>-0.1213273223639257</v>
+      </c>
+      <c r="F74" t="n">
+        <v>0.5374958362529944</v>
+      </c>
+      <c r="G74" t="n">
+        <v>0.90625</v>
+      </c>
+      <c r="H74" t="n">
+        <v>0.7179601737158342</v>
+      </c>
+      <c r="I74" t="n">
+        <v>0.9155986556322426</v>
+      </c>
+      <c r="J74" t="n">
+        <v>0.633669422315583</v>
+      </c>
+      <c r="K74" t="n">
+        <v>0.3806146572104019</v>
+      </c>
+      <c r="L74" t="inlineStr">
+        <is>
+          <t>opt</t>
+        </is>
+      </c>
+      <c r="M74" t="n">
+        <v>-0.02516555646033342</v>
+      </c>
+      <c r="N74" t="n">
+        <v>-0.2942140010088521</v>
+      </c>
+    </row>
+    <row r="75">
+      <c r="A75" t="inlineStr">
+        <is>
+          <t>bertopic</t>
+        </is>
+      </c>
+      <c r="B75" t="inlineStr">
+        <is>
+          <t>run_20250901T165942Z</t>
+        </is>
+      </c>
+      <c r="C75" t="inlineStr">
+        <is>
+          <t>trial_28</t>
+        </is>
+      </c>
+      <c r="D75" t="n">
+        <v>16</v>
+      </c>
+      <c r="E75" t="n">
+        <v>-0.1213273223639257</v>
+      </c>
+      <c r="F75" t="n">
+        <v>0.5374958362529944</v>
+      </c>
+      <c r="G75" t="n">
+        <v>0.90625</v>
+      </c>
+      <c r="H75" t="n">
+        <v>0.7179601737158342</v>
+      </c>
+      <c r="I75" t="n">
+        <v>0.9155986556322426</v>
+      </c>
+      <c r="J75" t="n">
+        <v>0.633669422315583</v>
+      </c>
+      <c r="K75" t="n">
+        <v>0.3806146572104019</v>
+      </c>
+      <c r="L75" t="inlineStr">
+        <is>
+          <t>opt</t>
+        </is>
+      </c>
+      <c r="M75" t="n">
+        <v>-0.02516555646033342</v>
+      </c>
+      <c r="N75" t="n">
+        <v>-0.2942140010088521</v>
+      </c>
+    </row>
+    <row r="76">
+      <c r="A76" t="inlineStr">
+        <is>
+          <t>bertopic</t>
+        </is>
+      </c>
+      <c r="B76" t="inlineStr">
+        <is>
+          <t>run_20250901T165942Z</t>
+        </is>
+      </c>
+      <c r="C76" t="inlineStr">
+        <is>
+          <t>trial_30</t>
+        </is>
+      </c>
+      <c r="D76" t="n">
+        <v>9</v>
+      </c>
+      <c r="E76" t="n">
+        <v>-0.03313921715550731</v>
+      </c>
+      <c r="F76" t="n">
+        <v>0.5819872846140995</v>
+      </c>
+      <c r="G76" t="n">
+        <v>0.8333333333333334</v>
+      </c>
+      <c r="H76" t="n">
+        <v>0.7697393194884969</v>
+      </c>
+      <c r="I76" t="n">
+        <v>0.929328096817758</v>
+      </c>
+      <c r="J76" t="n">
+        <v>0.6813184968077977</v>
+      </c>
+      <c r="K76" t="n">
+        <v>0.4964539007092199</v>
+      </c>
+      <c r="L76" t="inlineStr">
+        <is>
+          <t>opt</t>
+        </is>
+      </c>
+      <c r="M76" t="n">
+        <v>0.5393434208800163</v>
+      </c>
+      <c r="N76" t="n">
+        <v>0.3666431476213039</v>
+      </c>
+    </row>
+    <row r="77">
+      <c r="A77" t="inlineStr">
+        <is>
+          <t>bertopic</t>
+        </is>
+      </c>
+      <c r="B77" t="inlineStr">
+        <is>
+          <t>run_20250901T165942Z</t>
+        </is>
+      </c>
+      <c r="C77" t="inlineStr">
+        <is>
+          <t>trial_31</t>
+        </is>
+      </c>
+      <c r="D77" t="n">
+        <v>10</v>
+      </c>
+      <c r="E77" t="n">
+        <v>0.01129193678825731</v>
+      </c>
+      <c r="F77" t="n">
+        <v>0.6019632815671072</v>
+      </c>
+      <c r="G77" t="n">
+        <v>0.7</v>
+      </c>
+      <c r="H77" t="n">
+        <v>0.7622874507300536</v>
+      </c>
+      <c r="I77" t="n">
+        <v>0.9303286225796836</v>
+      </c>
+      <c r="J77" t="n">
+        <v>0.6232665061001467</v>
+      </c>
+      <c r="K77" t="n">
+        <v>0.2505910165484633</v>
+      </c>
+      <c r="L77" t="inlineStr">
+        <is>
+          <t>opt</t>
+        </is>
+      </c>
+      <c r="M77" t="n">
+        <v>0.5478810646321272</v>
+      </c>
+      <c r="N77" t="n">
+        <v>0.05436668472986758</v>
+      </c>
+    </row>
+    <row r="78">
+      <c r="A78" t="inlineStr">
+        <is>
+          <t>bertopic</t>
+        </is>
+      </c>
+      <c r="B78" t="inlineStr">
+        <is>
+          <t>run_20250901T165942Z</t>
+        </is>
+      </c>
+      <c r="C78" t="inlineStr">
+        <is>
+          <t>trial_34</t>
+        </is>
+      </c>
+      <c r="D78" t="n">
+        <v>23</v>
+      </c>
+      <c r="E78" t="inlineStr"/>
+      <c r="F78" t="n">
+        <v>0.624638980259887</v>
+      </c>
+      <c r="G78" t="n">
+        <v>0.8956521739130435</v>
+      </c>
+      <c r="H78" t="n">
+        <v>0.8066684192994791</v>
+      </c>
+      <c r="I78" t="n">
+        <v>0.9082709694501671</v>
+      </c>
+      <c r="J78" t="n">
+        <v>0.5281425942641254</v>
+      </c>
+      <c r="K78" t="n">
+        <v>0.3309692671394799</v>
+      </c>
+      <c r="L78" t="inlineStr">
+        <is>
+          <t>opt</t>
+        </is>
+      </c>
+      <c r="M78" t="inlineStr"/>
+      <c r="N78" t="n">
+        <v>-0.1960526923776497</v>
+      </c>
+    </row>
+    <row r="79">
+      <c r="A79" t="inlineStr">
+        <is>
+          <t>bertopic</t>
+        </is>
+      </c>
+      <c r="B79" t="inlineStr">
+        <is>
+          <t>run_20250901T165942Z</t>
+        </is>
+      </c>
+      <c r="C79" t="inlineStr">
+        <is>
+          <t>trial_35</t>
+        </is>
+      </c>
+      <c r="D79" t="n">
+        <v>27</v>
+      </c>
+      <c r="E79" t="inlineStr"/>
+      <c r="F79" t="n">
+        <v>0.5757428444168106</v>
+      </c>
+      <c r="G79" t="n">
+        <v>0.8777777777777778</v>
+      </c>
+      <c r="H79" t="n">
+        <v>0.8081805711675586</v>
+      </c>
+      <c r="I79" t="n">
+        <v>0.9402722504233937</v>
+      </c>
+      <c r="J79" t="n">
+        <v>0.6355190080443229</v>
+      </c>
+      <c r="K79" t="n">
+        <v>0.3617021276595745</v>
+      </c>
+      <c r="L79" t="inlineStr">
+        <is>
+          <t>opt</t>
+        </is>
+      </c>
+      <c r="M79" t="inlineStr"/>
+      <c r="N79" t="n">
+        <v>0.4900946425685736</v>
+      </c>
+    </row>
+    <row r="80">
+      <c r="A80" t="inlineStr">
+        <is>
+          <t>bertopic</t>
+        </is>
+      </c>
+      <c r="B80" t="inlineStr">
+        <is>
+          <t>run_20250901T165942Z</t>
+        </is>
+      </c>
+      <c r="C80" t="inlineStr">
+        <is>
+          <t>trial_36</t>
+        </is>
+      </c>
+      <c r="D80" t="n">
+        <v>22</v>
+      </c>
+      <c r="E80" t="n">
+        <v>-0.1969767018596764</v>
+      </c>
+      <c r="F80" t="n">
+        <v>0.5492427763828686</v>
+      </c>
+      <c r="G80" t="n">
+        <v>0.9045454545454545</v>
+      </c>
+      <c r="H80" t="n">
+        <v>0.735309471827342</v>
+      </c>
+      <c r="I80" t="n">
+        <v>0.9316726578961227</v>
+      </c>
+      <c r="J80" t="n">
+        <v>0.6779868665741433</v>
+      </c>
+      <c r="K80" t="n">
+        <v>0.2718676122931442</v>
+      </c>
+      <c r="L80" t="inlineStr">
+        <is>
+          <t>opt</t>
+        </is>
+      </c>
+      <c r="M80" t="n">
+        <v>-0.4454269686483028</v>
+      </c>
+      <c r="N80" t="n">
+        <v>0.1229804233241465</v>
+      </c>
+    </row>
+    <row r="81">
+      <c r="A81" t="inlineStr">
+        <is>
+          <t>bertopic</t>
+        </is>
+      </c>
+      <c r="B81" t="inlineStr">
+        <is>
+          <t>run_20250901T165942Z</t>
+        </is>
+      </c>
+      <c r="C81" t="inlineStr">
+        <is>
           <t>trial_39</t>
         </is>
       </c>
-      <c r="D58" t="n">
-        <v>12</v>
-      </c>
-      <c r="E58" t="n">
-        <v>0.009048572224704156</v>
-      </c>
-      <c r="F58" t="n">
-        <v>0.5948303152692596</v>
-      </c>
-      <c r="G58" t="n">
-        <v>0.7083333333333334</v>
-      </c>
-      <c r="H58" t="n">
-        <v>0.7916744452506473</v>
-      </c>
-      <c r="I58" t="n">
-        <v>0.9228149007779421</v>
-      </c>
-      <c r="J58" t="n">
-        <v>0.6453452726951627</v>
-      </c>
-      <c r="K58" t="n">
-        <v>0.2340425531914894</v>
-      </c>
-      <c r="L58" t="inlineStr">
-        <is>
-          <t>opt</t>
-        </is>
-      </c>
-      <c r="M58" t="n">
-        <v>0.5894196290453724</v>
-      </c>
-      <c r="N58" t="n">
-        <v>0.3286821940343204</v>
+      <c r="D81" t="n">
+        <v>14</v>
+      </c>
+      <c r="E81" t="n">
+        <v>-0.07967592265208649</v>
+      </c>
+      <c r="F81" t="n">
+        <v>0.5218152696612891</v>
+      </c>
+      <c r="G81" t="n">
+        <v>0.75</v>
+      </c>
+      <c r="H81" t="n">
+        <v>0.7942458868720299</v>
+      </c>
+      <c r="I81" t="n">
+        <v>0.9390647283946196</v>
+      </c>
+      <c r="J81" t="n">
+        <v>0.7307137816997692</v>
+      </c>
+      <c r="K81" t="n">
+        <v>0.2434988179669031</v>
+      </c>
+      <c r="L81" t="inlineStr">
+        <is>
+          <t>opt</t>
+        </is>
+      </c>
+      <c r="M81" t="n">
+        <v>-0.2678764870144701</v>
+      </c>
+      <c r="N81" t="n">
+        <v>0.82090262925798</v>
       </c>
     </row>
   </sheetData>

</xml_diff>